<commit_message>
Authoring code changes has beeen done
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -94,16 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">Validate Authoring functionalities like create, view and update </t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -503,15 +499,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -535,12 +531,10 @@
       <c r="B2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
@@ -549,12 +543,10 @@
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
@@ -595,10 +587,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -642,11 +634,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
adding changes to my local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -94,12 +94,25 @@
   </si>
   <si>
     <t xml:space="preserve">Validate Authoring functionalities like create, view and update </t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -499,15 +512,15 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -532,9 +545,11 @@
         <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
@@ -544,9 +559,11 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
@@ -556,9 +573,11 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
@@ -567,10 +586,12 @@
       <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,10 +608,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -634,11 +655,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
changes to my local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="4425"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="AuthoringTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="29">
   <si>
     <t>TCID</t>
   </si>
@@ -96,13 +97,10 @@
     <t xml:space="preserve">Validate Authoring functionalities like create, view and update </t>
   </si>
   <si>
+    <t>SKIP</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -512,7 +510,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -545,10 +543,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -559,10 +557,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -573,10 +571,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -586,11 +584,11 @@
       <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>27</v>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -600,7 +598,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>

</xml_diff>

<commit_message>
Taking back Chinna's changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -12,12 +12,11 @@
     <sheet name="AuthoringTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
   <si>
     <t>TCID</t>
   </si>
@@ -98,6 +97,15 @@
   </si>
   <si>
     <t>SKIP</t>
+  </si>
+  <si>
+    <t>AuthoringRecordViewDetailsTest</t>
+  </si>
+  <si>
+    <t>To verify Record View Details link Navigate to WOS page and Navigate to Project Neon Page</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>PASS</t>
@@ -507,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -557,7 +565,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -571,7 +579,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -585,9 +593,23 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -598,7 +620,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>

</xml_diff>

<commit_message>
Running suites c and d
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -103,12 +103,6 @@
   </si>
   <si>
     <t>To verify Record View Details link Navigate to WOS page and Navigate to Project Neon Page</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -118,7 +112,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -518,15 +511,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -554,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -565,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -579,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -593,7 +586,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -607,7 +600,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -628,10 +621,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -675,11 +668,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
taking latest code changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>TCID</t>
   </si>
@@ -103,12 +103,6 @@
   </si>
   <si>
     <t>To verify Record View Details link Navigate to WOS page and Navigate to Project Neon Page</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -118,7 +112,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -518,15 +511,15 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -554,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -565,7 +558,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>26</v>
@@ -579,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>26</v>
@@ -593,7 +586,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
@@ -607,7 +600,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -628,10 +621,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -675,11 +668,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Running Authoring test cases only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -1,18 +1,534 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
+    <sheet name="AuthoringTest" sheetId="5" r:id="rId3"/>
+  </sheets>
+  <calcPr calcId="125725"/>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>TC SCENARIO</t>
+  </si>
+  <si>
+    <t>TC STEPS</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>CompleteArticleName</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>chinna.putha@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>Welcome01</t>
+  </si>
+  <si>
+    <t>drug delivery System</t>
+  </si>
+  <si>
+    <t>Schizophrenia and drug delivery systems</t>
+  </si>
+  <si>
+    <t>Testing Comments</t>
+  </si>
+  <si>
+    <t>AuthoringTest</t>
+  </si>
+  <si>
+    <t>AuthoringDeleteTest</t>
+  </si>
+  <si>
+    <t>Delete Article comments and validate the count</t>
+  </si>
+  <si>
+    <t>AuthoringProfileCommentsTest</t>
+  </si>
+  <si>
+    <t>Validate Total Profile Comments</t>
+  </si>
+  <si>
+    <t>AuthoringAppreciateTest</t>
+  </si>
+  <si>
+    <t>To verify Authoring Comment Appreciation Functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Authoring functionalities like create, view and update </t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>AuthoringRecordViewDetailsTest</t>
+  </si>
+  <si>
+    <t>To verify Record View Details link Navigate to WOS page and Navigate to Project Neon Page</t>
+  </si>
+  <si>
+    <t>AuthoringPreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>To Verify Authoring prevent comment flooding by bots with same article</t>
+  </si>
+  <si>
+    <t>AuthoringDiffArticlePreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+</sst>
+</file>
+
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="4">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+  </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -54,7 +570,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -78,7 +594,7 @@
       <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -99,8 +615,37 @@
         <v>26</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="45">
+      <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="45">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -114,10 +659,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -161,11 +706,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
Taking latest code changes and updating new scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -10,13 +10,16 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
     <sheet name="AuthoringTest" sheetId="5" r:id="rId3"/>
+    <sheet name="CommentsMinMaxValidationTest" sheetId="6" r:id="rId4"/>
+    <sheet name="CommentsProfanityWordsCheckTest" sheetId="7" r:id="rId5"/>
+    <sheet name="UnsupportedTagsCommentsTest" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -54,9 +57,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>chinna.putha@thomsonreuters.com</t>
   </si>
   <si>
@@ -114,15 +114,118 @@
     <t>AuthoringDiffArticlePreventBotsCommentsTest</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>CommentsMinMaxValidationTest</t>
+  </si>
+  <si>
+    <t>Authoring comment min length and max length validation</t>
+  </si>
+  <si>
+    <t>minCharCount</t>
+  </si>
+  <si>
+    <t>expMinComment</t>
+  </si>
+  <si>
+    <t>maxCharCount</t>
+  </si>
+  <si>
+    <t>expMaxComment</t>
+  </si>
+  <si>
+    <t>Comments must have at least two characters. Please edit your comment.</t>
+  </si>
+  <si>
+    <t>You've reached the maximum length for comments.</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>CommentsProfanityWordsCheckTest</t>
+  </si>
+  <si>
+    <t>Authroing Article Comment Validation with Profanity words</t>
+  </si>
+  <si>
+    <t>profanityWords</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>finger fuck</t>
+  </si>
+  <si>
+    <t>Words we do not allow in comments have been masked.</t>
+  </si>
+  <si>
+    <t>mackprofanity</t>
+  </si>
+  <si>
+    <t>bastard</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>doosh fatass</t>
+  </si>
+  <si>
+    <t>mother fuck</t>
+  </si>
+  <si>
+    <t>bloody bitch</t>
+  </si>
+  <si>
+    <t>Authoring comment unsupported html tag validation</t>
+  </si>
+  <si>
+    <t>UnsupportedTagsCommentsTest</t>
+  </si>
+  <si>
+    <t>HTMLTags</t>
+  </si>
+  <si>
+    <t>ErrorMessage</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;This is a Heading&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Adding comment with Strong tag&lt;/strong&gt;</t>
+  </si>
+  <si>
+    <t>Unsupported formatting and tags are not allowed in comments.</t>
+  </si>
+  <si>
+    <t>&lt;li&gt;Coffee&lt;/li&gt;
+&lt;li&gt;Tea&lt;/li&gt;
+&lt;li&gt;Milk&lt;/li&gt;</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://www.w3schools.com"&gt;This is a link&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>ShareArticleOnTwitterTest</t>
+  </si>
+  <si>
+    <t>Article Sharing on Twitter</t>
+  </si>
+  <si>
+    <t>ShareArticleOnLITest</t>
+  </si>
+  <si>
+    <t>Article Sharing on Facebook</t>
+  </si>
+  <si>
+    <t>ShareArticleOnFBTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +254,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,8 +280,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,11 +316,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -219,6 +377,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,18 +713,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -548,103 +743,347 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="C4" s="10" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="10" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30">
+      <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="45">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="B9" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="22"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="22"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="23"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="18"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="18"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="18"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="18"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="18"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="18"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="18"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="18"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="18"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="18"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="18"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="18"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="18"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="18"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
     </row>
   </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="C20:C25"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="D32:D37"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -660,10 +1099,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -702,16 +1141,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -734,29 +1174,300 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="12">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1600</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="13" customFormat="1">
+      <c r="A1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="45">
+      <c r="A4" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
running only one shareArticleLITest.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -715,8 +715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -847,7 +847,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D9" s="30" t="s">
         <v>25</v>
@@ -885,7 +885,7 @@
         <v>41</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>25</v>
@@ -899,7 +899,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>25</v>
@@ -937,10 +937,10 @@
         <v>62</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -984,7 +984,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1025,7 +1025,7 @@
         <v>64</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
runnig whole authoring testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
   <si>
     <t>TCID</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>You've reached the maximum length for comments.</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>CommentsProfanityWordsCheckTest</t>
@@ -386,9 +383,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -414,6 +408,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -749,7 +746,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>25</v>
@@ -763,7 +760,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>25</v>
@@ -777,7 +774,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>25</v>
@@ -791,7 +788,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>25</v>
@@ -805,7 +802,7 @@
         <v>27</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>25</v>
@@ -819,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>25</v>
@@ -833,244 +830,236 @@
         <v>29</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="22"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="22"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="22"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="23"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C14" s="10" t="s">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="18" t="s">
+      <c r="B15" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="18"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="18"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="18"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="18"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="C20" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="29"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="18" t="s">
+      <c r="B26" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="29"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="29"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="29"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="29"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="29"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="18"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="18"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="18"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="18"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="18"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="18"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="18"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="18"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="A34" s="29"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="18"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="18"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="18"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="D9:D13"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
     <mergeCell ref="B20:B25"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="C20:C25"/>
@@ -1083,6 +1072,14 @@
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="C26:C31"/>
     <mergeCell ref="D26:D31"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="D9:D13"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1174,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1281,10 +1278,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="13" customFormat="1">
       <c r="A1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>2</v>
@@ -1295,86 +1292,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1401,10 +1398,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>2</v>
@@ -1415,58 +1412,58 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>58</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new test to Suite C.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="125">
   <si>
     <t>TCID</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>OPQA-309</t>
+  </si>
+  <si>
+    <t>CreateAndPublishPost</t>
+  </si>
+  <si>
+    <t>OPQA-360</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post and publish it.</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -495,7 +507,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -535,6 +547,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -830,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A27" sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1336,6 +1349,23 @@
       </c>
       <c r="E29" s="16" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1368,9 +1398,10 @@
     <hyperlink ref="B27" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
     <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
     <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId29"/>
+  <pageSetup orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new tests for Authoring-Post
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -16,14 +16,16 @@
     <sheet name="EditCommentProfanityWordChkTesT" sheetId="9" r:id="rId7"/>
     <sheet name="EditCommentMinMaxValidationTest" sheetId="10" r:id="rId8"/>
     <sheet name="UnsupportedTagsEditCommentsTest" sheetId="11" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="12" r:id="rId10"/>
+    <sheet name="MinMaxLengthValidationPostTitle" sheetId="12" r:id="rId10"/>
+    <sheet name="MinMaxLenValidationPostContent" sheetId="13" r:id="rId11"/>
+    <sheet name="PostProfanityWordCheckTest" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="144">
   <si>
     <t>TCID</t>
   </si>
@@ -210,9 +212,6 @@
     <t>VerifyFlagInUserComments</t>
   </si>
   <si>
-    <t>EditCommentMinMaxValidationTest</t>
-  </si>
-  <si>
     <t>EditCommentProfanityWordChkTest</t>
   </si>
   <si>
@@ -243,9 +242,6 @@
     <t>Verify that default comments displayed for an article is 10 and valildate more functionality</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that more button is not displayed for comments less than 10 </t>
-  </si>
-  <si>
     <t>Verify that user is able to flag and unflag the comments</t>
   </si>
   <si>
@@ -282,12 +278,6 @@
     <t>Verify that user is able to add an article on LinkedIn</t>
   </si>
   <si>
-    <t>Verify that profanity words are not allowed while editing the comments.</t>
-  </si>
-  <si>
-    <t>Verify that  proper error messages are diplayed for min and max length validation for editing the comments</t>
-  </si>
-  <si>
     <t>Verify that  proper error messages are diplayed for min and max length validation for creating the comments</t>
   </si>
   <si>
@@ -397,6 +387,75 @@
   </si>
   <si>
     <t>Verify that user is able to create a post and publish it.</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>MinMaxLengthValidationPostTitle</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post title</t>
+  </si>
+  <si>
+    <t>OPQA-361</t>
+  </si>
+  <si>
+    <t>OPQA-363</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post content</t>
+  </si>
+  <si>
+    <t>contentMinError</t>
+  </si>
+  <si>
+    <t>contentMaxError</t>
+  </si>
+  <si>
+    <t>Posts must have at least two characters. Please edit your post.</t>
+  </si>
+  <si>
+    <t>You've reached the maximum length for posts.</t>
+  </si>
+  <si>
+    <t>MinMaxLenValidationPostContent</t>
+  </si>
+  <si>
+    <t>titleMinError</t>
+  </si>
+  <si>
+    <t>Titles must have at least two characters. Please edit your title.</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOwnPost</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their own post</t>
+  </si>
+  <si>
+    <t>OPQA-379|OPQA-381</t>
+  </si>
+  <si>
+    <t>PostTitleProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>Words we do not allow in posts have been masked.</t>
+  </si>
+  <si>
+    <t>PostContentProfanityWordChkTest</t>
+  </si>
+  <si>
+    <t>EditPostContentProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post title</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post content</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that profanity words are not allowed in post content</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -843,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A27" sqref="A1:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A28" sqref="A1:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -863,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>1</v>
@@ -880,16 +939,16 @@
         <v>17</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30">
@@ -897,16 +956,16 @@
         <v>20</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30">
@@ -914,16 +973,16 @@
         <v>18</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30">
@@ -931,16 +990,16 @@
         <v>19</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
@@ -948,16 +1007,16 @@
         <v>21</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
@@ -965,16 +1024,16 @@
         <v>22</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30">
@@ -982,16 +1041,16 @@
         <v>23</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30">
@@ -999,16 +1058,16 @@
         <v>24</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1016,16 +1075,16 @@
         <v>31</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30">
@@ -1033,16 +1092,16 @@
         <v>42</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1050,16 +1109,16 @@
         <v>50</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1067,16 +1126,16 @@
         <v>51</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1084,16 +1143,16 @@
         <v>52</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1101,16 +1160,16 @@
         <v>53</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1118,16 +1177,16 @@
         <v>54</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1135,16 +1194,16 @@
         <v>55</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1152,16 +1211,16 @@
         <v>56</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30">
@@ -1169,16 +1228,16 @@
         <v>57</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1186,16 +1245,16 @@
         <v>58</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30">
@@ -1203,16 +1262,16 @@
         <v>59</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1220,152 +1279,254 @@
         <v>60</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D23" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30">
       <c r="A25" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="30">
       <c r="A26" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D27" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30">
       <c r="A28" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30">
       <c r="A29" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B31" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="D30" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>38</v>
+      <c r="C34" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1399,122 +1560,246 @@
     <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
     <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
     <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B34" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B35" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B36" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="47.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>210</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>10010</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4">
+        <v>34</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75">
+      <c r="A3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4">
+        <v>37</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75">
+      <c r="A6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>72</v>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75">
+      <c r="A7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1640,7 +1925,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1678,8 +1963,8 @@
       <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="10">
-        <v>1600</v>
+      <c r="C2" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>30</v>
@@ -2029,7 +2314,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2065,7 +2350,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10">
         <v>1600</v>

</xml_diff>

<commit_message>
Added new test to Authoring suite.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="152">
   <si>
     <t>TCID</t>
   </si>
@@ -474,6 +474,15 @@
   </si>
   <si>
     <t>EDIT POST:Verfiy that proper error messages are displyed for min max length validation of POST CONTENT</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-342|OPQA-359</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
   </si>
 </sst>
 </file>
@@ -916,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1587,6 +1596,21 @@
         <v>3</v>
       </c>
       <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added new methods to ProfilePage and PostRecordViewPage
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -483,12 +483,22 @@
   </si>
   <si>
     <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
+  </si>
+  <si>
+    <t>CreateAndEditPost</t>
+  </si>
+  <si>
+    <t>OPQA-382|OPQA-388|OPQA-406|OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -925,19 +935,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="17" customFormat="1">
@@ -1611,6 +1621,23 @@
         <v>3</v>
       </c>
       <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1651,9 +1678,10 @@
     <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
     <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
     <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -1667,8 +1695,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1721,11 +1749,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1784,9 +1812,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1894,21 +1922,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1918,21 +1946,294 @@
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="196.5" customHeight="1">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="196.5" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="252.75" customHeight="1">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="252.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,20 +2242,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2000,6 +2301,285 @@
         <v>3</v>
       </c>
       <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2008,19 +2588,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2062,6 +2642,285 @@
       <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2071,21 +2930,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1">
+    <row r="1" spans="1:5" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -2098,8 +2957,9 @@
       <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2112,8 +2972,9 @@
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="14" t="s">
         <v>36</v>
       </c>
@@ -2126,8 +2987,9 @@
       <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -2140,8 +3002,9 @@
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2154,8 +3017,9 @@
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
@@ -2168,8 +3032,9 @@
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
@@ -2182,6 +3047,251 @@
       <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2199,10 +3309,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2276,9 +3386,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2394,10 +3504,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2455,10 +3565,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Adding new Test Cases F6 and F7 in Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -483,12 +483,22 @@
   </si>
   <si>
     <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
+  </si>
+  <si>
+    <t>CreateAndEditPost</t>
+  </si>
+  <si>
+    <t>OPQA-382|OPQA-388|OPQA-406|OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -925,19 +935,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.48828125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="17" customFormat="1">
@@ -1611,6 +1621,23 @@
         <v>3</v>
       </c>
       <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1651,9 +1678,10 @@
     <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
     <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
     <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -1667,8 +1695,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1721,11 +1749,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1784,9 +1812,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1894,21 +1922,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1918,21 +1946,294 @@
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="48" customHeight="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="196.5" customHeight="1">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="196.5" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="252.75" customHeight="1">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="252.75" customHeight="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,20 +2242,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2000,6 +2301,285 @@
         <v>3</v>
       </c>
       <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2008,19 +2588,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2062,6 +2642,285 @@
       <c r="F2" s="1" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2071,21 +2930,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B44" sqref="A43:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1">
+    <row r="1" spans="1:5" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -2098,8 +2957,9 @@
       <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75">
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -2112,8 +2972,9 @@
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="14" t="s">
         <v>36</v>
       </c>
@@ -2126,8 +2987,9 @@
       <c r="D3" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
@@ -2140,8 +3002,9 @@
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2154,8 +3017,9 @@
       <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="8" t="s">
         <v>40</v>
       </c>
@@ -2168,8 +3032,9 @@
       <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="8" t="s">
         <v>41</v>
       </c>
@@ -2182,6 +3047,251 @@
       <c r="D7" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2199,10 +3309,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2276,9 +3386,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2394,10 +3504,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2455,10 +3565,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Updated Suite C excel
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -183,13 +183,322 @@
   </si>
   <si>
     <t>Words we do not allow in posts have been masked.</t>
+  </si>
+  <si>
+    <t>AuthoringAppreciateTest</t>
+  </si>
+  <si>
+    <t>OPQA-284</t>
+  </si>
+  <si>
+    <t>Verfiy that user can appreciate comments made by other neon users and validate appreciation count</t>
+  </si>
+  <si>
+    <t>AuthoringDeleteTest</t>
+  </si>
+  <si>
+    <t>OPQA-286</t>
+  </si>
+  <si>
+    <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
+  </si>
+  <si>
+    <t>AuthoringProfileCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-296</t>
+  </si>
+  <si>
+    <t>Verify that comments added by the neon user are listed in profile page of the user</t>
+  </si>
+  <si>
+    <t>AuthoringRecordViewDetailsTest</t>
+  </si>
+  <si>
+    <t>OPQA-299</t>
+  </si>
+  <si>
+    <t>Verify that details link in article record view is redirected to full record view of WOS</t>
+  </si>
+  <si>
+    <t>AuthoringPreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-275</t>
+  </si>
+  <si>
+    <t>Verify that prevention of comment flooding by bots with same article works as expected</t>
+  </si>
+  <si>
+    <t>AuthoringDiffArticlePreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>Verify that prevention of comment flooding by bots with different articles works as expected</t>
+  </si>
+  <si>
+    <t>CommentsMinMaxValidationTest</t>
+  </si>
+  <si>
+    <t>OPQA-242</t>
+  </si>
+  <si>
+    <t>Verify that  proper error messages are diplayed for min and max length validation for creating the comments</t>
+  </si>
+  <si>
+    <t>CommentsProfanityWordsCheckTest</t>
+  </si>
+  <si>
+    <t>OPQA-238</t>
+  </si>
+  <si>
+    <t>Verify that profanity words are not allowed while creating the comments.</t>
+  </si>
+  <si>
+    <t>UnsupportedTagsCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-248</t>
+  </si>
+  <si>
+    <t>Verify  that user can not add unsupported html tags while adding the comments</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>ShareArticleOnTwitterTest</t>
+  </si>
+  <si>
+    <t>OPQA-302</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on Twitter</t>
+  </si>
+  <si>
+    <t>ShareArticleOnLITest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on LinkedIn</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>ShareArticleOnFBTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on Facebook</t>
+  </si>
+  <si>
+    <t>VerifyCancelFlagAction</t>
+  </si>
+  <si>
+    <t>OPQA-473</t>
+  </si>
+  <si>
+    <t>Verify that user is able to cancel the flag action</t>
+  </si>
+  <si>
+    <t>VerifyCancelUnflagAction</t>
+  </si>
+  <si>
+    <t>OPQA-476</t>
+  </si>
+  <si>
+    <t>Verify that user is able to cancel the remove flag action</t>
+  </si>
+  <si>
+    <t>VerifyFlagUserComment</t>
+  </si>
+  <si>
+    <t>Verify that user is able to flag and unflag the comments</t>
+  </si>
+  <si>
+    <t>VerifyFlagActionWithoutReason</t>
+  </si>
+  <si>
+    <t>Veirfy that user cannot flag a comment without selecting a reason</t>
+  </si>
+  <si>
+    <t>VerifyFlagForCommentUserAuthoredThemselves</t>
+  </si>
+  <si>
+    <t>Verify that flag button is not displyed for comments a user authored themselves</t>
+  </si>
+  <si>
+    <t>VerifyFlagSetByOtherUsers</t>
+  </si>
+  <si>
+    <t>Verify that only the user who set the flag can see the comment has flagged</t>
+  </si>
+  <si>
+    <t>VerifyUnflagActionWithoutReason</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to unflag the comment without selecting a Reason</t>
+  </si>
+  <si>
+    <t>VerifyFlagInUserComments</t>
+  </si>
+  <si>
+    <t>Verify that flag button is displayed for comments</t>
+  </si>
+  <si>
+    <t>AuthoringAppreciateOwnCommentTest</t>
+  </si>
+  <si>
+    <t>OPQA-281</t>
+  </si>
+  <si>
+    <t>Verfiy that user can appreciate their own comment validate appreciation count</t>
+  </si>
+  <si>
+    <t>EditCommentProfanityWordChkTest</t>
+  </si>
+  <si>
+    <t>OPQA-240</t>
+  </si>
+  <si>
+    <t>Verify that profanity words are not allowed while editing the comments</t>
+  </si>
+  <si>
+    <t>VerifyEditOtherUsersComments</t>
+  </si>
+  <si>
+    <t>OPQA-271</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to edit and delete the comment added by other users</t>
+  </si>
+  <si>
+    <t>UnsupportedTagsEditCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-251</t>
+  </si>
+  <si>
+    <t>Verify  that user can not add unsupported html tags while editing the comments</t>
+  </si>
+  <si>
+    <t>VerifyMoreButtonComments</t>
+  </si>
+  <si>
+    <t>OPQA-305</t>
+  </si>
+  <si>
+    <t>Verify that more button is not displayed for comments less than 10</t>
+  </si>
+  <si>
+    <t>VerifyMoreFunctionalityForComments</t>
+  </si>
+  <si>
+    <t>Verify that default comments displayed for an article is 10 and valildate more functionality</t>
+  </si>
+  <si>
+    <t>VerifyCommenterDetails</t>
+  </si>
+  <si>
+    <t>OPQA-309</t>
+  </si>
+  <si>
+    <t>Verify that commenter details is diplayed in the comment and clicking on name redirects to the user's profile</t>
+  </si>
+  <si>
+    <t>CreateAndPublishPost</t>
+  </si>
+  <si>
+    <t>OPQA-360</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post and publish it.</t>
+  </si>
+  <si>
+    <t>MinMaxLengthValidationPostTitle</t>
+  </si>
+  <si>
+    <t>OPQA-361</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post title</t>
+  </si>
+  <si>
+    <t>MinMaxLenValidationPostContent</t>
+  </si>
+  <si>
+    <t>OPQA-363</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post content</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOwnPost</t>
+  </si>
+  <si>
+    <t>OPQA-379|OPQA-381</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their own post</t>
+  </si>
+  <si>
+    <t>PostTitleProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post title</t>
+  </si>
+  <si>
+    <t>PostContentProfanityWordChkTest</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post content</t>
+  </si>
+  <si>
+    <t>EditPostContentProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that profanity words are not allowed in post content</t>
+  </si>
+  <si>
+    <t>EditPostTitleProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that profanity words are not allowed in post title</t>
+  </si>
+  <si>
+    <t>EditPostTitleMinMaxLengthValidation</t>
+  </si>
+  <si>
+    <t>EDIT POST: Verfiy that proper error messages are displyed for min max length validation of post title</t>
+  </si>
+  <si>
+    <t>EidtPostContentMinMaxLenValidation</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that proper error messages are displyed for min max length validation of POST CONTENT</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-342|OPQA-359</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
+  </si>
+  <si>
+    <t>CreateAndEditPost</t>
+  </si>
+  <si>
+    <t>OPQA-382|OPQA-388|OPQA-406|OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +536,28 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -289,7 +620,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -314,16 +645,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,46 +970,738 @@
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" s="16" customFormat="1">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:5" ht="25.5">
+      <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5">
+      <c r="A3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.5">
+      <c r="A4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="25.5">
+      <c r="A7" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.5">
+      <c r="A8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.5">
+      <c r="A9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5">
+      <c r="A28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5">
+      <c r="A29" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5">
+      <c r="A31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5">
+      <c r="A32" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="1:5" ht="25.5">
+      <c r="A38" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" spans="1:5" ht="25.5">
+      <c r="A39" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
+    <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B13" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B14" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B15" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B19" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B20" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B22" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B16" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
+    <hyperlink ref="B21" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
+    <hyperlink ref="B18" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B34" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B35" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B36" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -1089,7 +2115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Taking updated code and adding TestCase_E7 & TestCase_E8
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -183,13 +183,322 @@
   </si>
   <si>
     <t>Words we do not allow in posts have been masked.</t>
+  </si>
+  <si>
+    <t>AuthoringAppreciateTest</t>
+  </si>
+  <si>
+    <t>OPQA-284</t>
+  </si>
+  <si>
+    <t>Verfiy that user can appreciate comments made by other neon users and validate appreciation count</t>
+  </si>
+  <si>
+    <t>AuthoringDeleteTest</t>
+  </si>
+  <si>
+    <t>OPQA-286</t>
+  </si>
+  <si>
+    <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
+  </si>
+  <si>
+    <t>AuthoringProfileCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-296</t>
+  </si>
+  <si>
+    <t>Verify that comments added by the neon user are listed in profile page of the user</t>
+  </si>
+  <si>
+    <t>AuthoringRecordViewDetailsTest</t>
+  </si>
+  <si>
+    <t>OPQA-299</t>
+  </si>
+  <si>
+    <t>Verify that details link in article record view is redirected to full record view of WOS</t>
+  </si>
+  <si>
+    <t>AuthoringPreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-275</t>
+  </si>
+  <si>
+    <t>Verify that prevention of comment flooding by bots with same article works as expected</t>
+  </si>
+  <si>
+    <t>AuthoringDiffArticlePreventBotsCommentsTest</t>
+  </si>
+  <si>
+    <t>Verify that prevention of comment flooding by bots with different articles works as expected</t>
+  </si>
+  <si>
+    <t>CommentsMinMaxValidationTest</t>
+  </si>
+  <si>
+    <t>OPQA-242</t>
+  </si>
+  <si>
+    <t>Verify that  proper error messages are diplayed for min and max length validation for creating the comments</t>
+  </si>
+  <si>
+    <t>CommentsProfanityWordsCheckTest</t>
+  </si>
+  <si>
+    <t>OPQA-238</t>
+  </si>
+  <si>
+    <t>Verify that profanity words are not allowed while creating the comments.</t>
+  </si>
+  <si>
+    <t>UnsupportedTagsCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-248</t>
+  </si>
+  <si>
+    <t>Verify  that user can not add unsupported html tags while adding the comments</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>ShareArticleOnTwitterTest</t>
+  </si>
+  <si>
+    <t>OPQA-302</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on Twitter</t>
+  </si>
+  <si>
+    <t>ShareArticleOnLITest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on LinkedIn</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>ShareArticleOnFBTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add an article on Facebook</t>
+  </si>
+  <si>
+    <t>VerifyCancelFlagAction</t>
+  </si>
+  <si>
+    <t>OPQA-473</t>
+  </si>
+  <si>
+    <t>Verify that user is able to cancel the flag action</t>
+  </si>
+  <si>
+    <t>VerifyCancelUnflagAction</t>
+  </si>
+  <si>
+    <t>OPQA-476</t>
+  </si>
+  <si>
+    <t>Verify that user is able to cancel the remove flag action</t>
+  </si>
+  <si>
+    <t>VerifyFlagUserComment</t>
+  </si>
+  <si>
+    <t>Verify that user is able to flag and unflag the comments</t>
+  </si>
+  <si>
+    <t>VerifyFlagActionWithoutReason</t>
+  </si>
+  <si>
+    <t>Veirfy that user cannot flag a comment without selecting a reason</t>
+  </si>
+  <si>
+    <t>VerifyFlagForCommentUserAuthoredThemselves</t>
+  </si>
+  <si>
+    <t>Verify that flag button is not displyed for comments a user authored themselves</t>
+  </si>
+  <si>
+    <t>VerifyFlagSetByOtherUsers</t>
+  </si>
+  <si>
+    <t>Verify that only the user who set the flag can see the comment has flagged</t>
+  </si>
+  <si>
+    <t>VerifyUnflagActionWithoutReason</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to unflag the comment without selecting a Reason</t>
+  </si>
+  <si>
+    <t>VerifyFlagInUserComments</t>
+  </si>
+  <si>
+    <t>Verify that flag button is displayed for comments</t>
+  </si>
+  <si>
+    <t>AuthoringAppreciateOwnCommentTest</t>
+  </si>
+  <si>
+    <t>OPQA-281</t>
+  </si>
+  <si>
+    <t>Verfiy that user can appreciate their own comment validate appreciation count</t>
+  </si>
+  <si>
+    <t>EditCommentProfanityWordChkTest</t>
+  </si>
+  <si>
+    <t>OPQA-240</t>
+  </si>
+  <si>
+    <t>Verify that profanity words are not allowed while editing the comments</t>
+  </si>
+  <si>
+    <t>VerifyEditOtherUsersComments</t>
+  </si>
+  <si>
+    <t>OPQA-271</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to edit and delete the comment added by other users</t>
+  </si>
+  <si>
+    <t>UnsupportedTagsEditCommentsTest</t>
+  </si>
+  <si>
+    <t>OPQA-251</t>
+  </si>
+  <si>
+    <t>Verify  that user can not add unsupported html tags while editing the comments</t>
+  </si>
+  <si>
+    <t>VerifyMoreButtonComments</t>
+  </si>
+  <si>
+    <t>OPQA-305</t>
+  </si>
+  <si>
+    <t>Verify that more button is not displayed for comments less than 10</t>
+  </si>
+  <si>
+    <t>VerifyMoreFunctionalityForComments</t>
+  </si>
+  <si>
+    <t>Verify that default comments displayed for an article is 10 and valildate more functionality</t>
+  </si>
+  <si>
+    <t>VerifyCommenterDetails</t>
+  </si>
+  <si>
+    <t>OPQA-309</t>
+  </si>
+  <si>
+    <t>Verify that commenter details is diplayed in the comment and clicking on name redirects to the user's profile</t>
+  </si>
+  <si>
+    <t>CreateAndPublishPost</t>
+  </si>
+  <si>
+    <t>OPQA-360</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create a post and publish it.</t>
+  </si>
+  <si>
+    <t>MinMaxLengthValidationPostTitle</t>
+  </si>
+  <si>
+    <t>OPQA-361</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post title</t>
+  </si>
+  <si>
+    <t>MinMaxLenValidationPostContent</t>
+  </si>
+  <si>
+    <t>OPQA-363</t>
+  </si>
+  <si>
+    <t>Verfiy that proper error messages are displyed for min max length validation of post content</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOwnPost</t>
+  </si>
+  <si>
+    <t>OPQA-379|OPQA-381</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their own post</t>
+  </si>
+  <si>
+    <t>PostTitleProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post title</t>
+  </si>
+  <si>
+    <t>PostContentProfanityWordChkTest</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that profanity words are not allowed in post content</t>
+  </si>
+  <si>
+    <t>EditPostContentProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that profanity words are not allowed in post content</t>
+  </si>
+  <si>
+    <t>EditPostTitleProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that profanity words are not allowed in post title</t>
+  </si>
+  <si>
+    <t>EditPostTitleMinMaxLengthValidation</t>
+  </si>
+  <si>
+    <t>EDIT POST: Verfiy that proper error messages are displyed for min max length validation of post title</t>
+  </si>
+  <si>
+    <t>EidtPostContentMinMaxLenValidation</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that proper error messages are displyed for min max length validation of POST CONTENT</t>
+  </si>
+  <si>
+    <t>AppreciateUnAppreciateOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-342|OPQA-359</t>
+  </si>
+  <si>
+    <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
+  </si>
+  <si>
+    <t>CreateAndEditPost</t>
+  </si>
+  <si>
+    <t>OPQA-382|OPQA-388|OPQA-406|OPQA-372</t>
+  </si>
+  <si>
+    <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +536,28 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -289,7 +620,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -314,16 +645,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -621,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -636,46 +970,738 @@
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" s="16" customFormat="1">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:5" ht="25.5">
+      <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="16" t="s">
+      <c r="D2" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="25.5">
+      <c r="A3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.5">
+      <c r="A4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="25.5">
+      <c r="A7" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="25.5">
+      <c r="A8" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="25.5">
+      <c r="A9" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="25.5">
+      <c r="A28" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="25.5">
+      <c r="A29" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="25.5">
+      <c r="A31" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="25.5">
+      <c r="A32" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="1:5" ht="25.5">
+      <c r="A38" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="18"/>
+    </row>
+    <row r="39" spans="1:5" ht="25.5">
+      <c r="A39" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
+    <hyperlink ref="B3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
+    <hyperlink ref="B4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
+    <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
+    <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
+    <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B13" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B14" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B15" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B19" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B20" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B22" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B16" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
+    <hyperlink ref="B21" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
+    <hyperlink ref="B18" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B34" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B35" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B36" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
@@ -1089,7 +2115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the data and locators
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Welcome01</t>
   </si>
   <si>
-    <t>drug delivery System</t>
-  </si>
-  <si>
     <t>Schizophrenia and drug delivery systems</t>
   </si>
   <si>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
+  </si>
+  <si>
+    <t>drug delivery SySchizophrenia and drug delivery systemsstem</t>
   </si>
 </sst>
 </file>
@@ -957,7 +957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:E41"/>
     </sheetView>
   </sheetViews>
@@ -975,7 +975,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -989,608 +989,608 @@
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>57</v>
-      </c>
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>60</v>
-      </c>
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="C6" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>63</v>
-      </c>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>66</v>
-      </c>
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>68</v>
-      </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>71</v>
-      </c>
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>74</v>
-      </c>
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="D11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>81</v>
-      </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="18" t="s">
+      <c r="D13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>83</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>86</v>
-      </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="C16" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>92</v>
-      </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>94</v>
-      </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>96</v>
-      </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>98</v>
-      </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>100</v>
-      </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>102</v>
-      </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>110</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="C25" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="C26" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="18" t="s">
-        <v>116</v>
-      </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="C29" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="D29" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B30" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="C30" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>127</v>
-      </c>
       <c r="D30" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="18" t="s">
-        <v>130</v>
-      </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="C32" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="C32" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="18" t="s">
-        <v>136</v>
-      </c>
       <c r="D33" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>138</v>
-      </c>
       <c r="D34" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>140</v>
-      </c>
       <c r="D35" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="D36" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>144</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>3</v>
@@ -1599,13 +1599,13 @@
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>146</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>3</v>
@@ -1614,13 +1614,13 @@
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="18" t="s">
         <v>147</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>148</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>3</v>
@@ -1629,13 +1629,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="C40" s="18" t="s">
         <v>150</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>151</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
@@ -1644,19 +1644,19 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B41" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="18" t="s">
-        <v>154</v>
-      </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1721,13 +1721,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1750,7 +1750,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1778,16 +1778,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1813,7 +1813,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1839,10 +1839,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -1853,86 +1853,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1985,8 +1985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2019,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2030,13 +2030,13 @@
         <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>3</v>
@@ -2067,16 +2067,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2090,19 +2090,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2129,10 +2129,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -2143,86 +2143,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2249,10 +2249,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -2263,44 +2263,44 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2325,10 +2325,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -2339,86 +2339,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2444,16 +2444,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2467,19 +2467,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="10">
         <v>1600</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2505,10 +2505,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>35</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -2519,44 +2519,44 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>38</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the test scripts.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
     <t>Verify that user is able to create and edit post and verify that time stamp is displayed</t>
   </si>
   <si>
-    <t>drug delivery SySchizophrenia and drug delivery systemsstem</t>
+    <t>drug delivery systems</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -655,9 +655,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -957,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,7 +964,7 @@
     <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -1018,7 +1015,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
@@ -1035,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1052,7 +1049,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1069,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
@@ -1086,7 +1083,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
@@ -1103,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
@@ -1120,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1137,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1154,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1171,7 +1168,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1205,7 +1202,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1222,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1239,7 +1236,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>29</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1456,7 +1453,7 @@
       <c r="C29" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
@@ -1473,7 +1470,7 @@
       <c r="C30" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
@@ -1507,7 +1504,7 @@
       <c r="C32" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
@@ -1524,7 +1521,7 @@
       <c r="C33" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
@@ -1541,7 +1538,7 @@
       <c r="C34" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
@@ -1558,7 +1555,7 @@
       <c r="C35" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
@@ -1575,7 +1572,7 @@
       <c r="C36" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
@@ -1592,7 +1589,7 @@
       <c r="C37" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18"/>
@@ -1607,7 +1604,7 @@
       <c r="C38" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18"/>
@@ -1622,7 +1619,7 @@
       <c r="C39" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="18"/>
@@ -1985,7 +1982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2029,7 +2026,7 @@
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="7" t="s">
         <v>154</v>
       </c>
       <c r="D2" s="7" t="s">

</xml_diff>

<commit_message>
Updated the authoring test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="153">
   <si>
     <t>TCID</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Verify  that user can not add unsupported html tags while adding the comments</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>ShareArticleOnTwitterTest</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
   </si>
   <si>
     <t>Verify that user is able to add an article on LinkedIn</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
   <si>
     <t>ShareArticleOnFBTest</t>
@@ -954,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D41"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -997,9 +991,7 @@
       <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
@@ -1014,9 +1006,7 @@
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
@@ -1031,9 +1021,7 @@
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
@@ -1048,9 +1036,7 @@
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
@@ -1065,9 +1051,7 @@
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
@@ -1082,9 +1066,7 @@
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E7" s="18"/>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
@@ -1099,9 +1081,7 @@
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
@@ -1116,9 +1096,7 @@
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
@@ -1133,9 +1111,7 @@
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
@@ -1150,444 +1126,392 @@
       <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>80</v>
-      </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>82</v>
-      </c>
       <c r="D13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E14" s="18"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>88</v>
-      </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>91</v>
-      </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E17" s="18"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E18" s="18"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E19" s="18"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E20" s="18"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E22" s="18"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>106</v>
-      </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>109</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E24" s="18"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>112</v>
-      </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E25" s="18"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>115</v>
-      </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E26" s="18"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E28" s="18"/>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>123</v>
-      </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="18" t="s">
-        <v>83</v>
-      </c>
+      <c r="E29" s="18"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>126</v>
-      </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E30" s="18"/>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E31" s="18"/>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>135</v>
-      </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E35" s="18"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>77</v>
-      </c>
+      <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
@@ -1596,13 +1520,13 @@
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
@@ -1611,13 +1535,13 @@
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
@@ -1626,13 +1550,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>148</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
@@ -1641,20 +1565,18 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>29</v>
-      </c>
+      <c r="E41" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2027,7 +1949,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Checked in New tests.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -486,6 +486,33 @@
   </si>
   <si>
     <t>drug delivery systems</t>
+  </si>
+  <si>
+    <t>VerifyPostRecordDetails</t>
+  </si>
+  <si>
+    <t>OPQA-370</t>
+  </si>
+  <si>
+    <t>Verify that user contributed articles display the information about the author</t>
+  </si>
+  <si>
+    <t>SeacrhAndViewOwnPost</t>
+  </si>
+  <si>
+    <t>OPQA-415</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search the  posts a user authored themselves and view them.</t>
+  </si>
+  <si>
+    <t>SeacrhAndViewOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-416</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search the posts of others and view them.</t>
   </si>
 </sst>
 </file>
@@ -946,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1577,6 +1604,57 @@
         <v>3</v>
       </c>
       <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
FIxing test cases fro watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="162">
   <si>
     <t>TCID</t>
   </si>
@@ -486,6 +486,33 @@
   </si>
   <si>
     <t>drug delivery systems</t>
+  </si>
+  <si>
+    <t>VerifyPostRecordDetails</t>
+  </si>
+  <si>
+    <t>OPQA-370</t>
+  </si>
+  <si>
+    <t>Verify that user contributed articles display the information about the author</t>
+  </si>
+  <si>
+    <t>SeacrhAndViewOwnPost</t>
+  </si>
+  <si>
+    <t>OPQA-415</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search the  posts a user authored themselves and view them.</t>
+  </si>
+  <si>
+    <t>SeacrhAndViewOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-416</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search the posts of others and view them.</t>
   </si>
 </sst>
 </file>
@@ -946,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1577,6 +1604,57 @@
         <v>3</v>
       </c>
       <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
2 search test cases added-B47 and B48
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="169">
   <si>
     <t>TCID</t>
   </si>
@@ -513,12 +513,34 @@
   </si>
   <si>
     <t>Verify that user is able to search the posts of others and view them.</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>CancelPostCreation</t>
+  </si>
+  <si>
+    <t>OPQA-376</t>
+  </si>
+  <si>
+    <t>Veirfy that user is able to cancel the post</t>
+  </si>
+  <si>
+    <t>CreatePostWithExternalLink</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to add external links to the post and publish it.</t>
+  </si>
+  <si>
+    <t>OPQA-367</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -641,7 +663,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -678,6 +700,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,19 +996,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -1603,7 +1626,9 @@
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="18"/>
+      <c r="E41" s="18" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
@@ -1636,7 +1661,7 @@
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>29</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1653,6 +1678,40 @@
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1712,8 +1771,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1766,11 +1825,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1829,9 +1888,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1947,10 +2006,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1988,12 +2047,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2055,11 +2114,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2118,10 +2177,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -2238,10 +2297,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2315,9 +2374,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2433,10 +2492,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2494,10 +2553,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Updated the excel.Added new test.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="189">
   <si>
     <t>TCID</t>
   </si>
@@ -293,9 +293,6 @@
     <t>VerifyCancelUnflagAction</t>
   </si>
   <si>
-    <t>OPQA-476</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the remove flag action</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>VerifyFlagInUserComments</t>
   </si>
   <si>
-    <t>Verify that flag button is displayed for comments</t>
-  </si>
-  <si>
     <t>AuthoringAppreciateOwnCommentTest</t>
   </si>
   <si>
@@ -410,18 +404,12 @@
     <t>OPQA-361</t>
   </si>
   <si>
-    <t>Verfiy that proper error messages are displyed for min max length validation of post title</t>
-  </si>
-  <si>
     <t>MinMaxLenValidationPostContent</t>
   </si>
   <si>
     <t>OPQA-363</t>
   </si>
   <si>
-    <t>Verfiy that proper error messages are displyed for min max length validation of post content</t>
-  </si>
-  <si>
     <t>AppreciateUnAppreciateOwnPost</t>
   </si>
   <si>
@@ -455,15 +443,9 @@
     <t>EditPostTitleMinMaxLengthValidation</t>
   </si>
   <si>
-    <t>EDIT POST: Verfiy that proper error messages are displyed for min max length validation of post title</t>
-  </si>
-  <si>
     <t>EidtPostContentMinMaxLenValidation</t>
   </si>
   <si>
-    <t>EDIT POST:Verfiy that proper error messages are displyed for min max length validation of POST CONTENT</t>
-  </si>
-  <si>
     <t>AppreciateUnAppreciateOthersPost</t>
   </si>
   <si>
@@ -546,13 +528,78 @@
   </si>
   <si>
     <t>PostContentProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>OPQA-1273</t>
+  </si>
+  <si>
+    <t>OPQA-1274</t>
+  </si>
+  <si>
+    <t>OPQA-1275</t>
+  </si>
+  <si>
+    <t>OPQA-1276</t>
+  </si>
+  <si>
+    <t>OPQA-1277</t>
+  </si>
+  <si>
+    <t>OPQA-1278</t>
+  </si>
+  <si>
+    <t>OPQA-1279</t>
+  </si>
+  <si>
+    <t>OPQA-1280</t>
+  </si>
+  <si>
+    <t>OPQA-1281</t>
+  </si>
+  <si>
+    <t>Verify that flag button is displayed for comments of other users</t>
+  </si>
+  <si>
+    <t>OPQA-1282</t>
+  </si>
+  <si>
+    <t>OPQA-1283</t>
+  </si>
+  <si>
+    <t>EDIT POST: Verfiy thatpublidh button is disabled when min and max length requirement for post title is not met.</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that publish button is disabled when min and max length requirement for post content is not met.</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that publish button is disabled when min and max length requirement for post title is not met.</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that publish button is disabled when min and max length requirement for post content is not met.</t>
+  </si>
+  <si>
+    <t>OPQA-1284</t>
+  </si>
+  <si>
+    <t>OPQA-1285</t>
+  </si>
+  <si>
+    <t>OPQA-1286</t>
+  </si>
+  <si>
+    <t>OPQA-1287</t>
+  </si>
+  <si>
+    <t>PQA-1288</t>
+  </si>
+  <si>
+    <t>OPQA-1289</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -675,7 +722,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -713,6 +760,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1010,17 +1058,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -1088,7 +1136,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1146,8 +1194,8 @@
       <c r="A8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>64</v>
+      <c r="B8" s="21" t="s">
+        <v>167</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>67</v>
@@ -1173,7 +1221,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1190,7 +1238,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1207,15 +1255,15 @@
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>78</v>
+      <c r="B12" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>79</v>
@@ -1224,15 +1272,15 @@
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>78</v>
+      <c r="B13" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>81</v>
@@ -1241,7 +1289,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1258,15 +1306,15 @@
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>85</v>
+      <c r="B15" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>86</v>
@@ -1275,273 +1323,273 @@
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>93</v>
-      </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>95</v>
-      </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>99</v>
-      </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>85</v>
+        <v>99</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>110</v>
-      </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>116</v>
-      </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="19" t="s">
         <v>115</v>
       </c>
+      <c r="B28" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="C28" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
@@ -1552,13 +1600,13 @@
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
@@ -1569,30 +1617,30 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>126</v>
+        <v>130</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
@@ -1603,13 +1651,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>129</v>
+        <v>166</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
@@ -1620,64 +1668,64 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>126</v>
+        <v>135</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>126</v>
+        <v>137</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>129</v>
+        <v>138</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
@@ -1686,132 +1734,132 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
@@ -1828,39 +1876,39 @@
     <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
     <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
     <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
-    <hyperlink ref="B10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
-    <hyperlink ref="B11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
-    <hyperlink ref="B12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B13" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B14" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B17" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B15" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B19" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B20" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B22" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B16" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
-    <hyperlink ref="B21" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
-    <hyperlink ref="B18" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B23" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
-    <hyperlink ref="B24" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
-    <hyperlink ref="B25" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
-    <hyperlink ref="B26" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
-    <hyperlink ref="B27" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
-    <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
-    <hyperlink ref="B31" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B32" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B34" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B35" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B36" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
-    <hyperlink ref="B47" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B9" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B14" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
+    <hyperlink ref="B47" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B8" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
+    <hyperlink ref="B13" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
+    <hyperlink ref="B12" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
+    <hyperlink ref="B15" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
+    <hyperlink ref="B16" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
+    <hyperlink ref="B18" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
+    <hyperlink ref="B19" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
+    <hyperlink ref="B20" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
+    <hyperlink ref="B21" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
+    <hyperlink ref="B22" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
+    <hyperlink ref="B28" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
+    <hyperlink ref="B34" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
+    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
+    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
+    <hyperlink ref="B35" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
+    <hyperlink ref="B36" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
+    <hyperlink ref="B39" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId40"/>
@@ -1877,8 +1925,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1931,11 +1979,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1994,9 +2042,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2112,10 +2160,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2153,12 +2201,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2192,7 +2240,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>
@@ -2220,11 +2268,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2283,10 +2331,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -2403,10 +2451,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2480,9 +2528,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2598,10 +2646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2659,10 +2707,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Adding new TestCase in Notifications
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="195">
   <si>
     <t>TCID</t>
   </si>
@@ -293,9 +293,6 @@
     <t>VerifyCancelUnflagAction</t>
   </si>
   <si>
-    <t>OPQA-476</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the remove flag action</t>
   </si>
   <si>
@@ -332,9 +329,6 @@
     <t>VerifyFlagInUserComments</t>
   </si>
   <si>
-    <t>Verify that flag button is displayed for comments</t>
-  </si>
-  <si>
     <t>AuthoringAppreciateOwnCommentTest</t>
   </si>
   <si>
@@ -410,18 +404,12 @@
     <t>OPQA-361</t>
   </si>
   <si>
-    <t>Verfiy that proper error messages are displyed for min max length validation of post title</t>
-  </si>
-  <si>
     <t>MinMaxLenValidationPostContent</t>
   </si>
   <si>
     <t>OPQA-363</t>
   </si>
   <si>
-    <t>Verfiy that proper error messages are displyed for min max length validation of post content</t>
-  </si>
-  <si>
     <t>AppreciateUnAppreciateOwnPost</t>
   </si>
   <si>
@@ -455,15 +443,9 @@
     <t>EditPostTitleMinMaxLengthValidation</t>
   </si>
   <si>
-    <t>EDIT POST: Verfiy that proper error messages are displyed for min max length validation of post title</t>
-  </si>
-  <si>
     <t>EidtPostContentMinMaxLenValidation</t>
   </si>
   <si>
-    <t>EDIT POST:Verfiy that proper error messages are displyed for min max length validation of POST CONTENT</t>
-  </si>
-  <si>
     <t>AppreciateUnAppreciateOthersPost</t>
   </si>
   <si>
@@ -546,6 +528,90 @@
   </si>
   <si>
     <t>PostContentProfanityWordCheckTest</t>
+  </si>
+  <si>
+    <t>OPQA-1273</t>
+  </si>
+  <si>
+    <t>OPQA-1274</t>
+  </si>
+  <si>
+    <t>OPQA-1275</t>
+  </si>
+  <si>
+    <t>OPQA-1276</t>
+  </si>
+  <si>
+    <t>OPQA-1277</t>
+  </si>
+  <si>
+    <t>OPQA-1278</t>
+  </si>
+  <si>
+    <t>OPQA-1279</t>
+  </si>
+  <si>
+    <t>OPQA-1280</t>
+  </si>
+  <si>
+    <t>OPQA-1281</t>
+  </si>
+  <si>
+    <t>Verify that flag button is displayed for comments of other users</t>
+  </si>
+  <si>
+    <t>OPQA-1282</t>
+  </si>
+  <si>
+    <t>OPQA-1283</t>
+  </si>
+  <si>
+    <t>EDIT POST: Verfiy thatpublidh button is disabled when min and max length requirement for post title is not met.</t>
+  </si>
+  <si>
+    <t>EDIT POST:Verfiy that publish button is disabled when min and max length requirement for post content is not met.</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that publish button is disabled when min and max length requirement for post title is not met.</t>
+  </si>
+  <si>
+    <t>CREATE POST:Verfiy that publish button is disabled when min and max length requirement for post content is not met.</t>
+  </si>
+  <si>
+    <t>OPQA-1284</t>
+  </si>
+  <si>
+    <t>OPQA-1285</t>
+  </si>
+  <si>
+    <t>OPQA-1286</t>
+  </si>
+  <si>
+    <t>OPQA-1287</t>
+  </si>
+  <si>
+    <t>PQA-1288</t>
+  </si>
+  <si>
+    <t>OPQA-1289</t>
+  </si>
+  <si>
+    <t>VerifyStatsOfOthersPost</t>
+  </si>
+  <si>
+    <t>OPQA-424|OPQA-426</t>
+  </si>
+  <si>
+    <t>Verify that user is able to view the comment and like counts on posts created by others</t>
+  </si>
+  <si>
+    <t>VerifyStatsOfOwnPost</t>
+  </si>
+  <si>
+    <t>OPQA-423|OPQA-425</t>
+  </si>
+  <si>
+    <t>Verify that user is able to view the comment and like counts on own posts</t>
   </si>
 </sst>
 </file>
@@ -675,7 +741,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -713,6 +779,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1008,10 +1078,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,7 +1158,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1146,8 +1216,8 @@
       <c r="A8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="19" t="s">
-        <v>64</v>
+      <c r="B8" s="21" t="s">
+        <v>167</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>67</v>
@@ -1173,7 +1243,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1190,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1207,15 +1277,15 @@
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="19" t="s">
-        <v>78</v>
+      <c r="B12" s="21" t="s">
+        <v>169</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>79</v>
@@ -1224,15 +1294,15 @@
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>78</v>
+      <c r="B13" s="21" t="s">
+        <v>168</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>81</v>
@@ -1241,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1258,15 +1328,15 @@
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>85</v>
+      <c r="B15" s="21" t="s">
+        <v>170</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>86</v>
@@ -1275,273 +1345,273 @@
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="18" t="s">
-        <v>89</v>
-      </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>93</v>
-      </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="B19" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>95</v>
-      </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>97</v>
-      </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>99</v>
-      </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>85</v>
+        <v>99</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>177</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>101</v>
+        <v>176</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>104</v>
-      </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>110</v>
-      </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>113</v>
-      </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>116</v>
-      </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="19" t="s">
         <v>115</v>
       </c>
+      <c r="B28" s="21" t="s">
+        <v>178</v>
+      </c>
       <c r="C28" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="B30" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>124</v>
-      </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>127</v>
+        <v>181</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
@@ -1552,13 +1622,13 @@
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
@@ -1569,30 +1639,30 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>126</v>
+        <v>130</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
@@ -1603,13 +1673,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>129</v>
+        <v>166</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>186</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
@@ -1620,64 +1690,64 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>129</v>
+        <v>133</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>187</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>126</v>
+        <v>135</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>126</v>
+        <v>137</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>129</v>
+        <v>138</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
@@ -1686,137 +1756,171 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1828,42 +1932,44 @@
     <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
     <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
     <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B8" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B9" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
-    <hyperlink ref="B10" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
-    <hyperlink ref="B11" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
-    <hyperlink ref="B12" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B13" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B14" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B17" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B15" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B19" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B20" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B22" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B16" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
-    <hyperlink ref="B21" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-476"/>
-    <hyperlink ref="B18" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B23" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
-    <hyperlink ref="B24" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
-    <hyperlink ref="B25" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
-    <hyperlink ref="B26" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
-    <hyperlink ref="B27" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B28" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B29" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
-    <hyperlink ref="B30" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
-    <hyperlink ref="B31" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B32" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B34" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B35" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B36" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B39" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B41" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
-    <hyperlink ref="B47" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B9" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B14" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
+    <hyperlink ref="B47" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B8" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
+    <hyperlink ref="B13" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
+    <hyperlink ref="B12" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
+    <hyperlink ref="B15" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
+    <hyperlink ref="B16" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
+    <hyperlink ref="B18" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
+    <hyperlink ref="B19" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
+    <hyperlink ref="B20" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
+    <hyperlink ref="B21" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
+    <hyperlink ref="B22" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
+    <hyperlink ref="B28" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
+    <hyperlink ref="B34" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
+    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
+    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
+    <hyperlink ref="B35" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
+    <hyperlink ref="B36" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
+    <hyperlink ref="B39" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
+    <hyperlink ref="B48" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
+    <hyperlink ref="B49" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -2192,7 +2298,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Committing for Suite C.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="221">
   <si>
     <t>TCID</t>
   </si>
@@ -524,9 +524,6 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>PostContentProfanityWordCheckTest</t>
   </si>
   <si>
@@ -630,13 +627,75 @@
   </si>
   <si>
     <t>OPQA-377</t>
+  </si>
+  <si>
+    <t>CommentOnOtherUsersPost</t>
+  </si>
+  <si>
+    <t>OPQA-385</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add comments on the posts of others.</t>
+  </si>
+  <si>
+    <t>ShareOthersPostInFB</t>
+  </si>
+  <si>
+    <t>ShareOthersPostOnLI</t>
+  </si>
+  <si>
+    <t>ShareOthersPostOnTwitter</t>
+  </si>
+  <si>
+    <t>ShareOwnPostInFB</t>
+  </si>
+  <si>
+    <t>ShareOwnPostOnLI</t>
+  </si>
+  <si>
+    <t>ShareOwnPostOnTwitter</t>
+  </si>
+  <si>
+    <t>OPQA-1307</t>
+  </si>
+  <si>
+    <t>OPQA-417</t>
+  </si>
+  <si>
+    <t>OPQA-1308</t>
+  </si>
+  <si>
+    <t>OPQA-418</t>
+  </si>
+  <si>
+    <t>OPQA-1309</t>
+  </si>
+  <si>
+    <t>OPQA-1310</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share the post created by others via FB</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share the post created by others via LI</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share the post created by others via Twitter</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share their posts on FB.</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share their posts on LI</t>
+  </si>
+  <si>
+    <t>Verify that user is able to share their posts on Twitter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -759,7 +818,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -798,9 +857,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1096,19 +1152,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:E51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
+    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -1142,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
@@ -1159,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
@@ -1176,7 +1232,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1193,7 +1249,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1210,7 +1266,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
@@ -1227,7 +1283,7 @@
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
@@ -1235,7 +1291,7 @@
         <v>66</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>67</v>
@@ -1244,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
@@ -1303,7 +1359,7 @@
         <v>77</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>79</v>
@@ -1320,7 +1376,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>81</v>
@@ -1354,7 +1410,7 @@
         <v>84</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>86</v>
@@ -1371,7 +1427,7 @@
         <v>87</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>88</v>
@@ -1405,7 +1461,7 @@
         <v>91</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>92</v>
@@ -1422,7 +1478,7 @@
         <v>93</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>94</v>
@@ -1439,7 +1495,7 @@
         <v>95</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>96</v>
@@ -1456,7 +1512,7 @@
         <v>97</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>98</v>
@@ -1473,10 +1529,10 @@
         <v>99</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
@@ -1575,7 +1631,7 @@
         <v>115</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>116</v>
@@ -1629,13 +1685,13 @@
         <v>124</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
@@ -1646,13 +1702,13 @@
         <v>126</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1669,7 +1725,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1677,7 +1733,7 @@
         <v>130</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>131</v>
@@ -1686,15 +1742,15 @@
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>132</v>
@@ -1703,7 +1759,7 @@
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1711,7 +1767,7 @@
         <v>133</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>134</v>
@@ -1728,7 +1784,7 @@
         <v>135</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>136</v>
@@ -1745,10 +1801,10 @@
         <v>137</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
@@ -1762,10 +1818,10 @@
         <v>138</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
@@ -1905,54 +1961,54 @@
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="C48" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="C49" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B50" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -1961,18 +2017,137 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="D51" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D51" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="B52" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2020,9 +2195,15 @@
     <hyperlink ref="B48" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
     <hyperlink ref="B49" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
     <hyperlink ref="B50" r:id="rId42" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-427"/>
+    <hyperlink ref="B57" r:id="rId43" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-417"/>
+    <hyperlink ref="B58" r:id="rId44" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1308"/>
+    <hyperlink ref="B56" r:id="rId45" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1307"/>
+    <hyperlink ref="B54" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
+    <hyperlink ref="B53" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
+    <hyperlink ref="B55" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId43"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
 
@@ -2036,8 +2217,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2090,11 +2271,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2153,9 +2334,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2271,10 +2452,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2312,12 +2493,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2379,11 +2560,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2442,10 +2623,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -2562,10 +2743,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2639,9 +2820,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2757,10 +2938,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2818,10 +2999,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Adding authoring Test case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="224">
   <si>
     <t>TCID</t>
   </si>
@@ -690,6 +690,15 @@
   </si>
   <si>
     <t>Verify that user is able to share their posts on Twitter</t>
+  </si>
+  <si>
+    <t>Verfify that user is able to save the post as a draft</t>
+  </si>
+  <si>
+    <t>OPQA-1195</t>
+  </si>
+  <si>
+    <t>VerifySavePostAsDraft</t>
   </si>
 </sst>
 </file>
@@ -818,7 +827,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -856,7 +865,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1152,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1290,7 +1298,7 @@
       <c r="A8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>166</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -1358,7 +1366,7 @@
       <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -1375,7 +1383,7 @@
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>167</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -1409,7 +1417,7 @@
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -1426,7 +1434,7 @@
       <c r="A16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>170</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -1460,7 +1468,7 @@
       <c r="A18" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>171</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -1477,7 +1485,7 @@
       <c r="A19" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>172</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -1494,7 +1502,7 @@
       <c r="A20" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>173</v>
       </c>
       <c r="C20" s="18" t="s">
@@ -1511,7 +1519,7 @@
       <c r="A21" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>174</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -1528,7 +1536,7 @@
       <c r="A22" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>176</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -1630,7 +1638,7 @@
       <c r="A28" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>177</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -1732,7 +1740,7 @@
       <c r="A34" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B34" s="20" t="s">
         <v>182</v>
       </c>
       <c r="C34" s="18" t="s">
@@ -1749,7 +1757,7 @@
       <c r="A35" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="20" t="s">
         <v>185</v>
       </c>
       <c r="C35" s="18" t="s">
@@ -1766,7 +1774,7 @@
       <c r="A36" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="20" t="s">
         <v>186</v>
       </c>
       <c r="C36" s="18" t="s">
@@ -1783,7 +1791,7 @@
       <c r="A37" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="20" t="s">
         <v>183</v>
       </c>
       <c r="C37" s="18" t="s">
@@ -1800,7 +1808,7 @@
       <c r="A38" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="20" t="s">
         <v>184</v>
       </c>
       <c r="C38" s="18" t="s">
@@ -1817,7 +1825,7 @@
       <c r="A39" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="20" t="s">
         <v>187</v>
       </c>
       <c r="C39" s="18" t="s">
@@ -1826,7 +1834,9 @@
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18"/>
+      <c r="E39" s="18" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
@@ -2012,7 +2022,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2029,7 +2039,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2063,7 +2073,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2080,7 +2090,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2097,7 +2107,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2114,7 +2124,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2148,6 +2158,23 @@
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test Cases for Authoring module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="227">
   <si>
     <t>TCID</t>
   </si>
@@ -699,6 +699,15 @@
   </si>
   <si>
     <t>VerifySavePostAsDraft</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
+  </si>
+  <si>
+    <t>OPQA-1312</t>
+  </si>
+  <si>
+    <t>VerifyAccessAndEditDraftPost</t>
   </si>
 </sst>
 </file>
@@ -827,7 +836,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -865,6 +874,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1160,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2175,6 +2187,23 @@
         <v>3</v>
       </c>
       <c r="E59" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding new test case to Authoring OPQA-1196
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
   <si>
     <t>TCID</t>
   </si>
@@ -695,9 +695,6 @@
     <t>Verfify that user is able to save the post as a draft</t>
   </si>
   <si>
-    <t>OPQA-1195</t>
-  </si>
-  <si>
     <t>VerifySavePostAsDraft</t>
   </si>
   <si>
@@ -708,6 +705,18 @@
   </si>
   <si>
     <t>VerifyAccessAndEditDraftPost</t>
+  </si>
+  <si>
+    <t>Verify that user is able to access and edit the draft posts from add a post modal</t>
+  </si>
+  <si>
+    <t>OPQA-1196</t>
+  </si>
+  <si>
+    <t>VerifyEditDraftPostFromModalWindow</t>
+  </si>
+  <si>
+    <t>OPQA-1195,OPQA-1313</t>
   </si>
 </sst>
 </file>
@@ -1172,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2175,10 +2184,10 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>221</v>
@@ -2192,18 +2201,35 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D60" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="8" t="s">
+      <c r="D61" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test cases for authoring
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="236">
   <si>
     <t>TCID</t>
   </si>
@@ -692,31 +692,49 @@
     <t>Verify that user is able to share their posts on Twitter</t>
   </si>
   <si>
+    <t>FlagUnflagUserPost</t>
+  </si>
+  <si>
+    <t>OPQA-1074|OPQA-1075</t>
+  </si>
+  <si>
+    <t>Verify that user is able to flag/unflag the posts of others.</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to delete their post</t>
+  </si>
+  <si>
+    <t> OPQA-1076</t>
+  </si>
+  <si>
+    <t>DeleteUserPost</t>
+  </si>
+  <si>
+    <t>VerifySavePostAsDraft</t>
+  </si>
+  <si>
+    <t>OPQA-1195,OPQA-1313</t>
+  </si>
+  <si>
     <t>Verfify that user is able to save the post as a draft</t>
   </si>
   <si>
-    <t>VerifySavePostAsDraft</t>
+    <t>VerifyAccessAndEditDraftPost</t>
+  </si>
+  <si>
+    <t>OPQA-1312</t>
   </si>
   <si>
     <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
   </si>
   <si>
-    <t>OPQA-1312</t>
-  </si>
-  <si>
-    <t>VerifyAccessAndEditDraftPost</t>
+    <t>VerifyEditDraftPostFromModalWindow</t>
+  </si>
+  <si>
+    <t>OPQA-1196</t>
   </si>
   <si>
     <t>Verify that user is able to access and edit the draft posts from add a post modal</t>
-  </si>
-  <si>
-    <t>OPQA-1196</t>
-  </si>
-  <si>
-    <t>VerifyEditDraftPostFromModalWindow</t>
-  </si>
-  <si>
-    <t>OPQA-1195,OPQA-1313</t>
   </si>
 </sst>
 </file>
@@ -845,7 +863,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -883,9 +901,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1181,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,7 +1339,7 @@
       <c r="A8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="21" t="s">
         <v>166</v>
       </c>
       <c r="C8" s="18" t="s">
@@ -1387,7 +1407,7 @@
       <c r="A12" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="21" t="s">
         <v>168</v>
       </c>
       <c r="C12" s="18" t="s">
@@ -1404,7 +1424,7 @@
       <c r="A13" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="21" t="s">
         <v>167</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -1438,7 +1458,7 @@
       <c r="A15" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -1455,7 +1475,7 @@
       <c r="A16" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="21" t="s">
         <v>170</v>
       </c>
       <c r="C16" s="18" t="s">
@@ -1489,7 +1509,7 @@
       <c r="A18" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>171</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -1506,7 +1526,7 @@
       <c r="A19" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="21" t="s">
         <v>172</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -1523,7 +1543,7 @@
       <c r="A20" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="21" t="s">
         <v>173</v>
       </c>
       <c r="C20" s="18" t="s">
@@ -1540,7 +1560,7 @@
       <c r="A21" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="21" t="s">
         <v>174</v>
       </c>
       <c r="C21" s="18" t="s">
@@ -1557,7 +1577,7 @@
       <c r="A22" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>176</v>
       </c>
       <c r="C22" s="18" t="s">
@@ -1659,7 +1679,7 @@
       <c r="A28" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="21" t="s">
         <v>177</v>
       </c>
       <c r="C28" s="18" t="s">
@@ -1761,7 +1781,7 @@
       <c r="A34" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="21" t="s">
         <v>182</v>
       </c>
       <c r="C34" s="18" t="s">
@@ -1778,7 +1798,7 @@
       <c r="A35" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="21" t="s">
         <v>185</v>
       </c>
       <c r="C35" s="18" t="s">
@@ -1795,7 +1815,7 @@
       <c r="A36" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="21" t="s">
         <v>186</v>
       </c>
       <c r="C36" s="18" t="s">
@@ -1812,7 +1832,7 @@
       <c r="A37" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="21" t="s">
         <v>183</v>
       </c>
       <c r="C37" s="18" t="s">
@@ -1829,7 +1849,7 @@
       <c r="A38" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="21" t="s">
         <v>184</v>
       </c>
       <c r="C38" s="18" t="s">
@@ -1846,7 +1866,7 @@
       <c r="A39" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="21" t="s">
         <v>187</v>
       </c>
       <c r="C39" s="18" t="s">
@@ -1855,9 +1875,7 @@
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>164</v>
-      </c>
+      <c r="E39" s="18"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
@@ -2043,7 +2061,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2060,7 +2078,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2094,7 +2112,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2111,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2128,7 +2146,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2145,7 +2163,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>164</v>
+        <v>29</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2184,52 +2202,86 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="C59" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D61" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" s="8" t="s">
+      <c r="D61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2283,9 +2335,11 @@
     <hyperlink ref="B54" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
     <hyperlink ref="B53" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
     <hyperlink ref="B55" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
+    <hyperlink ref="B59" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
+    <hyperlink ref="B60" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId49"/>
+  <pageSetup orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new tests to Suite C
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="242">
   <si>
     <t>TCID</t>
   </si>
@@ -632,9 +632,6 @@
     <t>CommentOnOtherUsersPost</t>
   </si>
   <si>
-    <t>OPQA-385</t>
-  </si>
-  <si>
     <t>Verify that user is able to add comments on the posts of others.</t>
   </si>
   <si>
@@ -745,6 +742,18 @@
   </si>
   <si>
     <t>VerifyDraftPostDisplayInUserOwnProfile</t>
+  </si>
+  <si>
+    <t>DeleteDraftPostFromProfile</t>
+  </si>
+  <si>
+    <t>OPQA-1090|OPQA-1201</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to delete the draft post from the list in their profile</t>
+  </si>
+  <si>
+    <t>OPQA-385|OPQA-364</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2094,10 +2103,10 @@
         <v>200</v>
       </c>
       <c r="B52" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>3</v>
@@ -2108,13 +2117,13 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>3</v>
@@ -2125,13 +2134,13 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>3</v>
@@ -2142,13 +2151,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>3</v>
@@ -2159,13 +2168,13 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
@@ -2176,13 +2185,13 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
@@ -2193,13 +2202,13 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
@@ -2210,13 +2219,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="C59" s="8" t="s">
         <v>222</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>223</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
@@ -2227,13 +2236,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
@@ -2244,13 +2253,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
@@ -2261,13 +2270,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>232</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
@@ -2278,13 +2287,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>235</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
@@ -2295,18 +2304,35 @@
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B64" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="8" t="s">
+      <c r="B65" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new test cases in suiteC
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -680,9 +680,6 @@
     <t>Verify that user is able to share the post created by others via Twitter</t>
   </si>
   <si>
-    <t>Verify that user is able to share their posts on FB.</t>
-  </si>
-  <si>
     <t>Verify that user is able to share their posts on LI</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>OPQA-385|OPQA-364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user is able to share their posts on FB. </t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2103,7 +2103,7 @@
         <v>200</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>201</v>
@@ -2174,7 +2174,7 @@
         <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
@@ -2191,7 +2191,7 @@
         <v>209</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
         <v>210</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
@@ -2219,13 +2219,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B59" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="C59" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>222</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
@@ -2236,13 +2236,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>228</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
@@ -2270,13 +2270,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>3</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Revert "Added new test cases in suiteC"
This reverts commit 3c2d097be97be27c457ed10e0e8d6ae0a0c8e387.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -680,6 +680,9 @@
     <t>Verify that user is able to share the post created by others via Twitter</t>
   </si>
   <si>
+    <t>Verify that user is able to share their posts on FB.</t>
+  </si>
+  <si>
     <t>Verify that user is able to share their posts on LI</t>
   </si>
   <si>
@@ -751,9 +754,6 @@
   </si>
   <si>
     <t>OPQA-385|OPQA-364</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user is able to share their posts on FB. </t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2103,7 +2103,7 @@
         <v>200</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>201</v>
@@ -2174,7 +2174,7 @@
         <v>208</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
@@ -2191,7 +2191,7 @@
         <v>209</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
@@ -2208,7 +2208,7 @@
         <v>210</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
@@ -2219,13 +2219,13 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
@@ -2236,13 +2236,13 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B60" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="C60" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
@@ -2253,13 +2253,13 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="21" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
@@ -2270,13 +2270,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="C64" s="4" t="s">
         <v>235</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>3</v>
@@ -2321,13 +2321,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Adding test case for Authoring module OPQA-1190
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="245">
   <si>
     <t>TCID</t>
   </si>
@@ -754,6 +754,16 @@
   </si>
   <si>
     <t>OPQA-385|OPQA-364</t>
+  </si>
+  <si>
+    <t>VerifyPublishPostDisplayed</t>
+  </si>
+  <si>
+    <t>OPQA-1190</t>
+  </si>
+  <si>
+    <t>Verify that Publish a Post option is displayed in Home page and all Record view 
+pages like Article,Post ,Patent</t>
   </si>
 </sst>
 </file>
@@ -1216,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2333,6 +2343,23 @@
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding test case for Authoring
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="248">
   <si>
     <t>TCID</t>
   </si>
@@ -764,6 +764,15 @@
   <si>
     <t>Verify that Publish a Post option is displayed in Home page and all Record view 
 pages like Article,Post ,Patent</t>
+  </si>
+  <si>
+    <t>Verfiy that the Drafts Post tab is not displayed when there are no draft posts</t>
+  </si>
+  <si>
+    <t>OPQA-1198</t>
+  </si>
+  <si>
+    <t>VerifyDraftPostTabDisplayForZeroDrafts</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2258,7 +2267,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2322,11 +2331,11 @@
       <c r="C64" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="D64" s="8" t="s">
+      <c r="D64" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>29</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2339,14 +2348,14 @@
       <c r="C65" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45">
       <c r="A66" s="1" t="s">
         <v>242</v>
       </c>
@@ -2356,10 +2365,27 @@
       <c r="C66" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the JIRA ID in Suite C excel.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -155,9 +155,6 @@
     <t>JIRA ID</t>
   </si>
   <si>
-    <t>OPQA-236</t>
-  </si>
-  <si>
     <t>1600</t>
   </si>
   <si>
@@ -185,18 +182,12 @@
     <t>AuthoringAppreciateTest</t>
   </si>
   <si>
-    <t>OPQA-284</t>
-  </si>
-  <si>
     <t>Verfiy that user can appreciate comments made by other neon users and validate appreciation count</t>
   </si>
   <si>
     <t>AuthoringDeleteTest</t>
   </si>
   <si>
-    <t>OPQA-286</t>
-  </si>
-  <si>
     <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t>VerifyCancelFlagAction</t>
   </si>
   <si>
-    <t>OPQA-473</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the flag action</t>
   </si>
   <si>
@@ -330,9 +318,6 @@
   </si>
   <si>
     <t>AuthoringAppreciateOwnCommentTest</t>
-  </si>
-  <si>
-    <t>OPQA-281</t>
   </si>
   <si>
     <t>Verfiy that user can appreciate their own comment validate appreciation count</t>
@@ -810,13 +795,28 @@
   </si>
   <si>
     <t>Verfiy that user is able to add links other NEON content [ex -Posts, articles, patents, profiles] to the comment</t>
+  </si>
+  <si>
+    <t>OPQA-475|OPQA-476</t>
+  </si>
+  <si>
+    <t>OPQA-286|OPQA-253</t>
+  </si>
+  <si>
+    <t>OPQA-236|OPQA-257</t>
+  </si>
+  <si>
+    <t>OPQA-281|OPQA-289</t>
+  </si>
+  <si>
+    <t>OPQA-284|OPQA-292</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +880,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -938,7 +944,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -977,6 +983,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1275,7 +1284,7 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1309,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>257</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>40</v>
@@ -1318,1140 +1327,1140 @@
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>55</v>
+        <v>256</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="19" t="s">
         <v>85</v>
       </c>
+      <c r="B17" s="22" t="s">
+        <v>255</v>
+      </c>
       <c r="C17" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>101</v>
+        <v>258</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="45">
       <c r="A66" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>3</v>
@@ -2462,13 +2471,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>3</v>
@@ -2479,13 +2488,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>3</v>
@@ -2496,56 +2505,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
-    <hyperlink ref="B4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
-    <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
-    <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
-    <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B9" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
-    <hyperlink ref="B10" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
-    <hyperlink ref="B11" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
-    <hyperlink ref="B14" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B17" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B23" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
-    <hyperlink ref="B24" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
-    <hyperlink ref="B25" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
-    <hyperlink ref="B26" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
-    <hyperlink ref="B27" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B29" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
-    <hyperlink ref="B30" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
-    <hyperlink ref="B31" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B32" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B41" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
-    <hyperlink ref="B47" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
-    <hyperlink ref="B8" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
-    <hyperlink ref="B13" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
-    <hyperlink ref="B12" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
-    <hyperlink ref="B15" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
-    <hyperlink ref="B16" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
-    <hyperlink ref="B18" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
-    <hyperlink ref="B19" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
-    <hyperlink ref="B20" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
-    <hyperlink ref="B21" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
-    <hyperlink ref="B22" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
-    <hyperlink ref="B28" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
-    <hyperlink ref="B34" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
-    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
-    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
-    <hyperlink ref="B35" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
-    <hyperlink ref="B36" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
-    <hyperlink ref="B39" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
-    <hyperlink ref="B48" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
-    <hyperlink ref="B49" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
-    <hyperlink ref="B50" r:id="rId42" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-427"/>
-    <hyperlink ref="B57" r:id="rId43" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-417"/>
-    <hyperlink ref="B58" r:id="rId44" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1308"/>
-    <hyperlink ref="B56" r:id="rId45" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1307"/>
-    <hyperlink ref="B54" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
-    <hyperlink ref="B53" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
-    <hyperlink ref="B55" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
-    <hyperlink ref="B59" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
-    <hyperlink ref="B60" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
+    <hyperlink ref="B6" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
+    <hyperlink ref="B7" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B9" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B14" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
+    <hyperlink ref="B47" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B8" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
+    <hyperlink ref="B13" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
+    <hyperlink ref="B12" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
+    <hyperlink ref="B15" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
+    <hyperlink ref="B16" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
+    <hyperlink ref="B18" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
+    <hyperlink ref="B19" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
+    <hyperlink ref="B20" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
+    <hyperlink ref="B21" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
+    <hyperlink ref="B22" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
+    <hyperlink ref="B28" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
+    <hyperlink ref="B34" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
+    <hyperlink ref="B37" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
+    <hyperlink ref="B38" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
+    <hyperlink ref="B35" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
+    <hyperlink ref="B36" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
+    <hyperlink ref="B39" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
+    <hyperlink ref="B48" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
+    <hyperlink ref="B49" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
+    <hyperlink ref="B50" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-427"/>
+    <hyperlink ref="B57" r:id="rId42" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-417"/>
+    <hyperlink ref="B58" r:id="rId43" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1308"/>
+    <hyperlink ref="B56" r:id="rId44" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1307"/>
+    <hyperlink ref="B54" r:id="rId45" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
+    <hyperlink ref="B53" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
+    <hyperlink ref="B55" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
+    <hyperlink ref="B59" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
+    <hyperlink ref="B60" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
+    <hyperlink ref="B2" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId51"/>
@@ -2568,7 +2577,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>17</v>
@@ -2585,7 +2594,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2625,10 +2634,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>17</v>
@@ -2645,10 +2654,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2703,7 +2712,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -2717,7 +2726,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -2731,7 +2740,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2745,7 +2754,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
@@ -2759,7 +2768,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
@@ -2773,7 +2782,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
@@ -2877,7 +2886,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>
@@ -2940,7 +2949,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Adding test case for notification
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="260">
   <si>
     <t>TCID</t>
   </si>
@@ -155,9 +155,6 @@
     <t>JIRA ID</t>
   </si>
   <si>
-    <t>OPQA-236</t>
-  </si>
-  <si>
     <t>1600</t>
   </si>
   <si>
@@ -185,18 +182,12 @@
     <t>AuthoringAppreciateTest</t>
   </si>
   <si>
-    <t>OPQA-284</t>
-  </si>
-  <si>
     <t>Verfiy that user can appreciate comments made by other neon users and validate appreciation count</t>
   </si>
   <si>
     <t>AuthoringDeleteTest</t>
   </si>
   <si>
-    <t>OPQA-286</t>
-  </si>
-  <si>
     <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
   </si>
   <si>
@@ -284,9 +275,6 @@
     <t>VerifyCancelFlagAction</t>
   </si>
   <si>
-    <t>OPQA-473</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the flag action</t>
   </si>
   <si>
@@ -330,9 +318,6 @@
   </si>
   <si>
     <t>AuthoringAppreciateOwnCommentTest</t>
-  </si>
-  <si>
-    <t>OPQA-281</t>
   </si>
   <si>
     <t>Verfiy that user can appreciate their own comment validate appreciation count</t>
@@ -792,13 +777,46 @@
   </si>
   <si>
     <t>VerifyPostTitleDisplayInDraftSection</t>
+  </si>
+  <si>
+    <t>AddExternalLinksToComments</t>
+  </si>
+  <si>
+    <t>OPQA-1092</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to add external links to the comment</t>
+  </si>
+  <si>
+    <t>AddInternalLinksToComments</t>
+  </si>
+  <si>
+    <t>OPQA-1093</t>
+  </si>
+  <si>
+    <t>Verfiy that user is able to add links other NEON content [ex -Posts, articles, patents, profiles] to the comment</t>
+  </si>
+  <si>
+    <t>OPQA-475|OPQA-476</t>
+  </si>
+  <si>
+    <t>OPQA-286|OPQA-253</t>
+  </si>
+  <si>
+    <t>OPQA-236|OPQA-257</t>
+  </si>
+  <si>
+    <t>OPQA-281|OPQA-289</t>
+  </si>
+  <si>
+    <t>OPQA-284|OPQA-292</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,6 +880,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -920,7 +944,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -959,6 +983,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1254,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1291,7 +1318,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>257</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>40</v>
@@ -1300,1140 +1327,1140 @@
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>55</v>
+        <v>256</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="19" t="s">
         <v>85</v>
       </c>
+      <c r="B17" s="22" t="s">
+        <v>255</v>
+      </c>
       <c r="C17" s="18" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>101</v>
+        <v>258</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D41" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D42" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D44" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D45" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D47" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D48" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D49" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D50" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D51" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D52" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D53" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D54" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D55" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D57" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D58" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D60" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="21" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D61" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D62" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D63" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="8" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D64" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D65" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="45">
       <c r="A66" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D66" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D68" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>3</v>
@@ -2442,58 +2469,92 @@
         <v>29</v>
       </c>
     </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
-    <hyperlink ref="B4" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
-    <hyperlink ref="B5" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
-    <hyperlink ref="B6" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
-    <hyperlink ref="B7" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
-    <hyperlink ref="B9" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
-    <hyperlink ref="B10" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
-    <hyperlink ref="B11" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
-    <hyperlink ref="B14" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
-    <hyperlink ref="B17" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
-    <hyperlink ref="B23" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
-    <hyperlink ref="B24" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
-    <hyperlink ref="B25" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
-    <hyperlink ref="B26" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
-    <hyperlink ref="B27" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
-    <hyperlink ref="B29" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
-    <hyperlink ref="B30" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
-    <hyperlink ref="B31" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
-    <hyperlink ref="B32" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
-    <hyperlink ref="B41" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
-    <hyperlink ref="B47" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
-    <hyperlink ref="B8" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
-    <hyperlink ref="B13" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
-    <hyperlink ref="B12" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
-    <hyperlink ref="B15" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
-    <hyperlink ref="B16" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
-    <hyperlink ref="B18" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
-    <hyperlink ref="B19" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
-    <hyperlink ref="B20" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
-    <hyperlink ref="B21" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
-    <hyperlink ref="B22" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
-    <hyperlink ref="B28" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
-    <hyperlink ref="B34" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
-    <hyperlink ref="B37" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
-    <hyperlink ref="B38" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
-    <hyperlink ref="B35" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
-    <hyperlink ref="B36" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
-    <hyperlink ref="B39" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
-    <hyperlink ref="B48" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
-    <hyperlink ref="B49" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
-    <hyperlink ref="B50" r:id="rId42" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-427"/>
-    <hyperlink ref="B57" r:id="rId43" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-417"/>
-    <hyperlink ref="B58" r:id="rId44" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1308"/>
-    <hyperlink ref="B56" r:id="rId45" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1307"/>
-    <hyperlink ref="B54" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
-    <hyperlink ref="B53" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
-    <hyperlink ref="B55" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
-    <hyperlink ref="B59" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
-    <hyperlink ref="B60" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
+    <hyperlink ref="B3" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-284"/>
+    <hyperlink ref="B4" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-286"/>
+    <hyperlink ref="B5" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-296"/>
+    <hyperlink ref="B6" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-299"/>
+    <hyperlink ref="B7" r:id="rId5" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-275"/>
+    <hyperlink ref="B9" r:id="rId6" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-242"/>
+    <hyperlink ref="B10" r:id="rId7" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-238"/>
+    <hyperlink ref="B11" r:id="rId8" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-248"/>
+    <hyperlink ref="B14" r:id="rId9" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-302"/>
+    <hyperlink ref="B17" r:id="rId10" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-473"/>
+    <hyperlink ref="B23" r:id="rId11" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-281"/>
+    <hyperlink ref="B24" r:id="rId12" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-240"/>
+    <hyperlink ref="B25" r:id="rId13" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-271"/>
+    <hyperlink ref="B26" r:id="rId14" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-251"/>
+    <hyperlink ref="B27" r:id="rId15" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-305"/>
+    <hyperlink ref="B29" r:id="rId16" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-309"/>
+    <hyperlink ref="B30" r:id="rId17" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-360"/>
+    <hyperlink ref="B31" r:id="rId18" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-361"/>
+    <hyperlink ref="B32" r:id="rId19" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-363"/>
+    <hyperlink ref="B41" r:id="rId20" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-382"/>
+    <hyperlink ref="B47" r:id="rId21" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-244"/>
+    <hyperlink ref="B8" r:id="rId22" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1273"/>
+    <hyperlink ref="B13" r:id="rId23" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1274"/>
+    <hyperlink ref="B12" r:id="rId24" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1275"/>
+    <hyperlink ref="B15" r:id="rId25" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1276"/>
+    <hyperlink ref="B16" r:id="rId26" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1277"/>
+    <hyperlink ref="B18" r:id="rId27" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1278"/>
+    <hyperlink ref="B19" r:id="rId28" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1279"/>
+    <hyperlink ref="B20" r:id="rId29" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1280"/>
+    <hyperlink ref="B21" r:id="rId30" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1281"/>
+    <hyperlink ref="B22" r:id="rId31" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1282"/>
+    <hyperlink ref="B28" r:id="rId32" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1283"/>
+    <hyperlink ref="B34" r:id="rId33" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1284"/>
+    <hyperlink ref="B37" r:id="rId34" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1285"/>
+    <hyperlink ref="B38" r:id="rId35" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1286"/>
+    <hyperlink ref="B35" r:id="rId36" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1287"/>
+    <hyperlink ref="B36" r:id="rId37" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1288"/>
+    <hyperlink ref="B39" r:id="rId38" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1289"/>
+    <hyperlink ref="B48" r:id="rId39" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-424"/>
+    <hyperlink ref="B49" r:id="rId40" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-423"/>
+    <hyperlink ref="B50" r:id="rId41" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-427"/>
+    <hyperlink ref="B57" r:id="rId42" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-417"/>
+    <hyperlink ref="B58" r:id="rId43" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1308"/>
+    <hyperlink ref="B56" r:id="rId44" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1307"/>
+    <hyperlink ref="B54" r:id="rId45" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-418"/>
+    <hyperlink ref="B53" r:id="rId46" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1309"/>
+    <hyperlink ref="B55" r:id="rId47" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1310"/>
+    <hyperlink ref="B59" r:id="rId48" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1074"/>
+    <hyperlink ref="B60" r:id="rId49" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-1076"/>
+    <hyperlink ref="B2" r:id="rId50" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-236"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId51"/>
@@ -2516,7 +2577,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>17</v>
@@ -2533,7 +2594,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2573,10 +2634,10 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>17</v>
@@ -2593,10 +2654,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2651,7 +2712,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -2665,7 +2726,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
@@ -2679,7 +2740,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -2693,7 +2754,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
@@ -2707,7 +2768,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
@@ -2721,7 +2782,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
@@ -2825,7 +2886,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>
@@ -2888,7 +2949,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Enabled only failing tests
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="261">
   <si>
     <t>TCID</t>
   </si>
@@ -810,6 +810,9 @@
   </si>
   <si>
     <t>OPQA-284|OPQA-292</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1324,7 +1327,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>159</v>
@@ -1341,7 +1344,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>159</v>
@@ -1358,7 +1361,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>159</v>
@@ -1375,7 +1378,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>159</v>
@@ -1392,7 +1395,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>159</v>
@@ -1409,7 +1412,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>159</v>
@@ -1426,7 +1429,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>159</v>
@@ -1443,7 +1446,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>159</v>
@@ -1460,7 +1463,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>159</v>
@@ -1477,7 +1480,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>159</v>
@@ -1511,7 +1514,7 @@
         <v>78</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>159</v>
@@ -1528,7 +1531,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>159</v>
@@ -1545,7 +1548,7 @@
         <v>82</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>159</v>
@@ -1562,7 +1565,7 @@
         <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>159</v>
@@ -1579,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>159</v>
@@ -1596,7 +1599,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>159</v>
@@ -1613,7 +1616,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>159</v>
@@ -1630,7 +1633,7 @@
         <v>92</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>159</v>
@@ -1647,7 +1650,7 @@
         <v>94</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>159</v>
@@ -1664,7 +1667,7 @@
         <v>170</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>159</v>
@@ -1681,7 +1684,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>159</v>
@@ -1698,7 +1701,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>159</v>
@@ -1715,7 +1718,7 @@
         <v>103</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>159</v>
@@ -1732,7 +1735,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>159</v>
@@ -1749,7 +1752,7 @@
         <v>109</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>159</v>
@@ -1766,7 +1769,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>159</v>
@@ -1783,7 +1786,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>159</v>
@@ -1800,7 +1803,7 @@
         <v>117</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>159</v>
@@ -1817,7 +1820,7 @@
         <v>175</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>159</v>
@@ -1834,7 +1837,7 @@
         <v>176</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>159</v>
@@ -1851,7 +1854,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>159</v>
@@ -1868,7 +1871,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>159</v>
@@ -1885,7 +1888,7 @@
         <v>127</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>159</v>
@@ -1902,7 +1905,7 @@
         <v>129</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>159</v>
@@ -1919,7 +1922,7 @@
         <v>131</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>159</v>
@@ -1936,7 +1939,7 @@
         <v>173</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>159</v>
@@ -1953,7 +1956,7 @@
         <v>174</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>159</v>
@@ -1970,7 +1973,7 @@
         <v>136</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>159</v>
@@ -1987,7 +1990,7 @@
         <v>139</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>159</v>
@@ -2004,7 +2007,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>159</v>
@@ -2021,7 +2024,7 @@
         <v>146</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>159</v>
@@ -2038,7 +2041,7 @@
         <v>149</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>159</v>
@@ -2055,7 +2058,7 @@
         <v>152</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>159</v>
@@ -2072,7 +2075,7 @@
         <v>154</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>159</v>
@@ -2089,7 +2092,7 @@
         <v>158</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>159</v>
@@ -2106,7 +2109,7 @@
         <v>185</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>159</v>
@@ -2123,7 +2126,7 @@
         <v>188</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>159</v>
@@ -2140,7 +2143,7 @@
         <v>190</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>159</v>
@@ -2157,7 +2160,7 @@
         <v>193</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>159</v>
@@ -2174,7 +2177,7 @@
         <v>196</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>159</v>
@@ -2191,7 +2194,7 @@
         <v>209</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>159</v>
@@ -2208,7 +2211,7 @@
         <v>210</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>159</v>
@@ -2242,7 +2245,7 @@
         <v>212</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>159</v>
@@ -2259,7 +2262,7 @@
         <v>213</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>159</v>
@@ -2279,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2293,7 +2296,7 @@
         <v>217</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>159</v>
@@ -2310,7 +2313,7 @@
         <v>218</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>159</v>
@@ -2327,7 +2330,7 @@
         <v>223</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>159</v>
@@ -2344,7 +2347,7 @@
         <v>226</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>159</v>
@@ -2361,7 +2364,7 @@
         <v>229</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>159</v>
@@ -2378,7 +2381,7 @@
         <v>230</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>159</v>
@@ -2395,7 +2398,7 @@
         <v>235</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>159</v>
@@ -2412,7 +2415,7 @@
         <v>239</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>159</v>
@@ -2429,7 +2432,7 @@
         <v>240</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>159</v>
@@ -2446,7 +2449,7 @@
         <v>245</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>159</v>
@@ -2463,10 +2466,10 @@
         <v>246</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2479,11 +2482,11 @@
       <c r="C70" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>3</v>
+      <c r="D70" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2496,11 +2499,11 @@
       <c r="C71" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>3</v>
+      <c r="D71" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
watch list script fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="261">
   <si>
     <t>TCID</t>
   </si>
@@ -810,6 +810,9 @@
   </si>
   <si>
     <t>OPQA-284|OPQA-292</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1324,7 +1327,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>159</v>
@@ -1341,7 +1344,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>159</v>
@@ -1358,7 +1361,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>159</v>
@@ -1375,7 +1378,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>159</v>
@@ -1392,7 +1395,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>159</v>
@@ -1409,7 +1412,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>159</v>
@@ -1426,7 +1429,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>159</v>
@@ -1443,7 +1446,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>159</v>
@@ -1460,7 +1463,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>159</v>
@@ -1477,7 +1480,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>159</v>
@@ -1511,7 +1514,7 @@
         <v>78</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>159</v>
@@ -1528,7 +1531,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>159</v>
@@ -1545,7 +1548,7 @@
         <v>82</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>159</v>
@@ -1562,7 +1565,7 @@
         <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>159</v>
@@ -1579,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>159</v>
@@ -1596,7 +1599,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>159</v>
@@ -1613,7 +1616,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>159</v>
@@ -1630,7 +1633,7 @@
         <v>92</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>159</v>
@@ -1647,7 +1650,7 @@
         <v>94</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>159</v>
@@ -1664,7 +1667,7 @@
         <v>170</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>159</v>
@@ -1681,7 +1684,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>159</v>
@@ -1698,7 +1701,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>159</v>
@@ -1715,7 +1718,7 @@
         <v>103</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>159</v>
@@ -1732,7 +1735,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>159</v>
@@ -1749,7 +1752,7 @@
         <v>109</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>159</v>
@@ -1766,7 +1769,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>159</v>
@@ -1783,7 +1786,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>159</v>
@@ -1800,7 +1803,7 @@
         <v>117</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>159</v>
@@ -1817,7 +1820,7 @@
         <v>175</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>159</v>
@@ -1834,7 +1837,7 @@
         <v>176</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>159</v>
@@ -1851,7 +1854,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>159</v>
@@ -1868,7 +1871,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>159</v>
@@ -1885,7 +1888,7 @@
         <v>127</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>159</v>
@@ -1902,7 +1905,7 @@
         <v>129</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>159</v>
@@ -1919,7 +1922,7 @@
         <v>131</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>159</v>
@@ -1936,7 +1939,7 @@
         <v>173</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>159</v>
@@ -1953,7 +1956,7 @@
         <v>174</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>159</v>
@@ -1970,7 +1973,7 @@
         <v>136</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>159</v>
@@ -1987,7 +1990,7 @@
         <v>139</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>159</v>
@@ -2004,7 +2007,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>159</v>
@@ -2021,7 +2024,7 @@
         <v>146</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>159</v>
@@ -2038,7 +2041,7 @@
         <v>149</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>159</v>
@@ -2055,7 +2058,7 @@
         <v>152</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>159</v>
@@ -2072,7 +2075,7 @@
         <v>154</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>159</v>
@@ -2089,7 +2092,7 @@
         <v>158</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>159</v>
@@ -2106,7 +2109,7 @@
         <v>185</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>159</v>
@@ -2123,7 +2126,7 @@
         <v>188</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>159</v>
@@ -2140,7 +2143,7 @@
         <v>190</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>159</v>
@@ -2157,7 +2160,7 @@
         <v>193</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>159</v>
@@ -2174,7 +2177,7 @@
         <v>196</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>159</v>
@@ -2191,7 +2194,7 @@
         <v>209</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>159</v>
@@ -2208,7 +2211,7 @@
         <v>210</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>159</v>
@@ -2242,7 +2245,7 @@
         <v>212</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>159</v>
@@ -2259,7 +2262,7 @@
         <v>213</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>159</v>
@@ -2279,7 +2282,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>159</v>
+        <v>29</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2293,7 +2296,7 @@
         <v>217</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>159</v>
@@ -2310,7 +2313,7 @@
         <v>218</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>159</v>
@@ -2327,7 +2330,7 @@
         <v>223</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>159</v>
@@ -2344,7 +2347,7 @@
         <v>226</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>159</v>
@@ -2361,7 +2364,7 @@
         <v>229</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>159</v>
@@ -2378,7 +2381,7 @@
         <v>230</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>159</v>
@@ -2395,7 +2398,7 @@
         <v>235</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>159</v>
@@ -2412,7 +2415,7 @@
         <v>239</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>159</v>
@@ -2429,7 +2432,7 @@
         <v>240</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>159</v>
@@ -2446,7 +2449,7 @@
         <v>245</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>159</v>
@@ -2463,10 +2466,10 @@
         <v>246</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>3</v>
+        <v>260</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2479,11 +2482,11 @@
       <c r="C70" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>3</v>
+      <c r="D70" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2496,11 +2499,11 @@
       <c r="C71" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>3</v>
+      <c r="D71" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>29</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled all test in Suite C
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="260">
   <si>
     <t>TCID</t>
   </si>
@@ -813,9 +813,6 @@
   </si>
   <si>
     <t>OPQA-284|OPQA-292</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1289,8 +1286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68:D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1330,7 +1327,7 @@
         <v>40</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
         <v>159</v>
@@ -1347,7 +1344,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>159</v>
@@ -1364,7 +1361,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>159</v>
@@ -1381,7 +1378,7 @@
         <v>56</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>159</v>
@@ -1398,7 +1395,7 @@
         <v>59</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>159</v>
@@ -1415,7 +1412,7 @@
         <v>62</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>159</v>
@@ -1432,7 +1429,7 @@
         <v>64</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>159</v>
@@ -1449,7 +1446,7 @@
         <v>67</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>159</v>
@@ -1466,7 +1463,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>159</v>
@@ -1483,7 +1480,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>159</v>
@@ -1517,7 +1514,7 @@
         <v>78</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>159</v>
@@ -1534,7 +1531,7 @@
         <v>80</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>159</v>
@@ -1551,7 +1548,7 @@
         <v>82</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>159</v>
@@ -1568,7 +1565,7 @@
         <v>84</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>159</v>
@@ -1585,7 +1582,7 @@
         <v>86</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>159</v>
@@ -1602,7 +1599,7 @@
         <v>88</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>159</v>
@@ -1619,7 +1616,7 @@
         <v>90</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>159</v>
@@ -1636,7 +1633,7 @@
         <v>92</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>159</v>
@@ -1653,7 +1650,7 @@
         <v>94</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>159</v>
@@ -1670,7 +1667,7 @@
         <v>170</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>159</v>
@@ -1687,7 +1684,7 @@
         <v>97</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>159</v>
@@ -1704,7 +1701,7 @@
         <v>100</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
         <v>159</v>
@@ -1721,7 +1718,7 @@
         <v>103</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
         <v>159</v>
@@ -1738,7 +1735,7 @@
         <v>106</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>159</v>
@@ -1755,7 +1752,7 @@
         <v>109</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
         <v>159</v>
@@ -1772,7 +1769,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
         <v>159</v>
@@ -1789,7 +1786,7 @@
         <v>114</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
         <v>159</v>
@@ -1806,7 +1803,7 @@
         <v>117</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>159</v>
@@ -1823,7 +1820,7 @@
         <v>175</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>159</v>
@@ -1840,7 +1837,7 @@
         <v>176</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
         <v>159</v>
@@ -1857,7 +1854,7 @@
         <v>124</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>159</v>
@@ -1874,7 +1871,7 @@
         <v>126</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
         <v>159</v>
@@ -1891,7 +1888,7 @@
         <v>127</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
         <v>159</v>
@@ -1908,7 +1905,7 @@
         <v>129</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
         <v>159</v>
@@ -1925,7 +1922,7 @@
         <v>131</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>159</v>
@@ -1942,7 +1939,7 @@
         <v>173</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>159</v>
@@ -1959,7 +1956,7 @@
         <v>174</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
         <v>159</v>
@@ -1976,7 +1973,7 @@
         <v>136</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
         <v>159</v>
@@ -1993,7 +1990,7 @@
         <v>139</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>159</v>
@@ -2010,7 +2007,7 @@
         <v>143</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>29</v>
@@ -2027,7 +2024,7 @@
         <v>146</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>159</v>
@@ -2044,7 +2041,7 @@
         <v>149</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>159</v>
@@ -2061,7 +2058,7 @@
         <v>152</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>159</v>
@@ -2078,7 +2075,7 @@
         <v>154</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>159</v>
@@ -2095,7 +2092,7 @@
         <v>158</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>159</v>
@@ -2112,7 +2109,7 @@
         <v>185</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>159</v>
@@ -2129,7 +2126,7 @@
         <v>188</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>159</v>
@@ -2146,7 +2143,7 @@
         <v>190</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>159</v>
@@ -2163,7 +2160,7 @@
         <v>193</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>159</v>
@@ -2180,7 +2177,7 @@
         <v>196</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>159</v>
@@ -2197,7 +2194,7 @@
         <v>209</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>159</v>
@@ -2214,7 +2211,7 @@
         <v>210</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>159</v>
@@ -2248,7 +2245,7 @@
         <v>212</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>159</v>
@@ -2265,7 +2262,7 @@
         <v>213</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>159</v>
@@ -2299,7 +2296,7 @@
         <v>217</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>159</v>
@@ -2316,7 +2313,7 @@
         <v>218</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>159</v>
@@ -2333,7 +2330,7 @@
         <v>223</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>159</v>
@@ -2350,7 +2347,7 @@
         <v>226</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>159</v>
@@ -2367,7 +2364,7 @@
         <v>229</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>159</v>
@@ -2384,7 +2381,7 @@
         <v>230</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>159</v>
@@ -2401,7 +2398,7 @@
         <v>235</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>159</v>
@@ -2418,7 +2415,7 @@
         <v>239</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>159</v>
@@ -2435,7 +2432,7 @@
         <v>240</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>159</v>
@@ -2452,7 +2449,7 @@
         <v>245</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>159</v>
@@ -2469,7 +2466,7 @@
         <v>246</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>159</v>
@@ -2486,7 +2483,7 @@
         <v>251</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>159</v>
@@ -2503,7 +2500,7 @@
         <v>254</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>260</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
changes in F1 and F2 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -1289,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changed module name and testcase name for Suite C
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -9,15 +9,15 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
-    <sheet name="AuthoringTest" sheetId="5" r:id="rId3"/>
-    <sheet name="CommentsMinMaxValidationTest" sheetId="6" r:id="rId4"/>
-    <sheet name="CommentsProfanityWordsCheckTest" sheetId="7" r:id="rId5"/>
-    <sheet name="UnsupportedTagsCommentsTest" sheetId="8" r:id="rId6"/>
-    <sheet name="EditCommentProfanityWordChkTesT" sheetId="9" r:id="rId7"/>
-    <sheet name="EditCommentMinMaxValidationTest" sheetId="10" r:id="rId8"/>
-    <sheet name="UnsupportedTagsEditCommentsTest" sheetId="11" r:id="rId9"/>
-    <sheet name="MinMaxLengthValidationPostTitle" sheetId="12" r:id="rId10"/>
-    <sheet name="MinMaxLenValidationPostContent" sheetId="13" r:id="rId11"/>
+    <sheet name="Authoring1" sheetId="5" r:id="rId3"/>
+    <sheet name="Authoring8" sheetId="6" r:id="rId4"/>
+    <sheet name="Authoring9" sheetId="7" r:id="rId5"/>
+    <sheet name="Authoring10" sheetId="8" r:id="rId6"/>
+    <sheet name="Authoring23" sheetId="9" r:id="rId7"/>
+    <sheet name="Authoring46" sheetId="10" r:id="rId8"/>
+    <sheet name="Authoring25" sheetId="11" r:id="rId9"/>
+    <sheet name="Authoring30" sheetId="12" r:id="rId10"/>
+    <sheet name="Authoring31" sheetId="13" r:id="rId11"/>
     <sheet name="PostProfanityWordCheckTest" sheetId="14" r:id="rId12"/>
   </sheets>
   <definedNames>
@@ -78,9 +78,6 @@
     <t>Testing Comments</t>
   </si>
   <si>
-    <t>AuthoringTest</t>
-  </si>
-  <si>
     <t>minCharCount</t>
   </si>
   <si>
@@ -182,270 +179,156 @@
     <t>Words we do not allow in posts have been masked.</t>
   </si>
   <si>
-    <t>AuthoringAppreciateTest</t>
-  </si>
-  <si>
     <t>Verfiy that user can appreciate comments made by other neon users and validate appreciation count</t>
   </si>
   <si>
-    <t>AuthoringDeleteTest</t>
-  </si>
-  <si>
     <t>Verify that user can delete the comments user authored themselves and validate the comment count</t>
   </si>
   <si>
-    <t>AuthoringProfileCommentsTest</t>
-  </si>
-  <si>
     <t>OPQA-296</t>
   </si>
   <si>
     <t>Verify that comments added by the neon user are listed in profile page of the user</t>
   </si>
   <si>
-    <t>AuthoringRecordViewDetailsTest</t>
-  </si>
-  <si>
     <t>OPQA-299</t>
   </si>
   <si>
     <t>Verify that details link in article record view is redirected to full record view of WOS</t>
   </si>
   <si>
-    <t>AuthoringPreventBotsCommentsTest</t>
-  </si>
-  <si>
     <t>OPQA-275</t>
   </si>
   <si>
     <t>Verify that prevention of comment flooding by bots with same article works as expected</t>
   </si>
   <si>
-    <t>AuthoringDiffArticlePreventBotsCommentsTest</t>
-  </si>
-  <si>
     <t>Verify that prevention of comment flooding by bots with different articles works as expected</t>
   </si>
   <si>
-    <t>CommentsMinMaxValidationTest</t>
-  </si>
-  <si>
     <t>OPQA-242</t>
   </si>
   <si>
     <t>Verify that  proper error messages are diplayed for min and max length validation for creating the comments</t>
   </si>
   <si>
-    <t>CommentsProfanityWordsCheckTest</t>
-  </si>
-  <si>
     <t>OPQA-238</t>
   </si>
   <si>
     <t>Verify that profanity words are not allowed while creating the comments.</t>
   </si>
   <si>
-    <t>UnsupportedTagsCommentsTest</t>
-  </si>
-  <si>
     <t>OPQA-248</t>
   </si>
   <si>
     <t>Verify  that user can not add unsupported html tags while adding the comments</t>
   </si>
   <si>
-    <t>ShareArticleOnTwitterTest</t>
-  </si>
-  <si>
     <t>OPQA-302</t>
   </si>
   <si>
     <t>Verify that user is able to add an article on Twitter</t>
   </si>
   <si>
-    <t>ShareArticleOnLITest</t>
-  </si>
-  <si>
     <t>Verify that user is able to add an article on LinkedIn</t>
   </si>
   <si>
-    <t>ShareArticleOnFBTest</t>
-  </si>
-  <si>
     <t>Verify that user is able to add an article on Facebook</t>
   </si>
   <si>
-    <t>VerifyCancelFlagAction</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the flag action</t>
   </si>
   <si>
-    <t>VerifyCancelUnflagAction</t>
-  </si>
-  <si>
     <t>Verify that user is able to cancel the remove flag action</t>
   </si>
   <si>
-    <t>VerifyFlagUserComment</t>
-  </si>
-  <si>
     <t>Verify that user is able to flag and unflag the comments</t>
   </si>
   <si>
-    <t>VerifyFlagActionWithoutReason</t>
-  </si>
-  <si>
     <t>Veirfy that user cannot flag a comment without selecting a reason</t>
   </si>
   <si>
-    <t>VerifyFlagForCommentUserAuthoredThemselves</t>
-  </si>
-  <si>
     <t>Verify that flag button is not displyed for comments a user authored themselves</t>
   </si>
   <si>
-    <t>VerifyFlagSetByOtherUsers</t>
-  </si>
-  <si>
     <t>Verify that only the user who set the flag can see the comment has flagged</t>
   </si>
   <si>
-    <t>VerifyUnflagActionWithoutReason</t>
-  </si>
-  <si>
     <t>Verify that user is not able to unflag the comment without selecting a Reason</t>
   </si>
   <si>
-    <t>VerifyFlagInUserComments</t>
-  </si>
-  <si>
-    <t>AuthoringAppreciateOwnCommentTest</t>
-  </si>
-  <si>
     <t>Verfiy that user can appreciate their own comment validate appreciation count</t>
   </si>
   <si>
-    <t>EditCommentProfanityWordChkTest</t>
-  </si>
-  <si>
     <t>OPQA-240</t>
   </si>
   <si>
     <t>Verify that profanity words are not allowed while editing the comments</t>
   </si>
   <si>
-    <t>VerifyEditOtherUsersComments</t>
-  </si>
-  <si>
     <t>OPQA-271</t>
   </si>
   <si>
     <t>Verify that user is not able to edit and delete the comment added by other users</t>
   </si>
   <si>
-    <t>UnsupportedTagsEditCommentsTest</t>
-  </si>
-  <si>
     <t>OPQA-251</t>
   </si>
   <si>
     <t>Verify  that user can not add unsupported html tags while editing the comments</t>
   </si>
   <si>
-    <t>VerifyMoreButtonComments</t>
-  </si>
-  <si>
     <t>OPQA-305</t>
   </si>
   <si>
     <t>Verify that more button is not displayed for comments less than 10</t>
   </si>
   <si>
-    <t>VerifyMoreFunctionalityForComments</t>
-  </si>
-  <si>
     <t>Verify that default comments displayed for an article is 10 and valildate more functionality</t>
   </si>
   <si>
-    <t>VerifyCommenterDetails</t>
-  </si>
-  <si>
     <t>OPQA-309</t>
   </si>
   <si>
     <t>Verify that commenter details is diplayed in the comment and clicking on name redirects to the user's profile</t>
   </si>
   <si>
-    <t>CreateAndPublishPost</t>
-  </si>
-  <si>
     <t>OPQA-360</t>
   </si>
   <si>
     <t>Verify that user is able to create a post and publish it.</t>
   </si>
   <si>
-    <t>MinMaxLengthValidationPostTitle</t>
-  </si>
-  <si>
     <t>OPQA-361</t>
   </si>
   <si>
-    <t>MinMaxLenValidationPostContent</t>
-  </si>
-  <si>
     <t>OPQA-363</t>
   </si>
   <si>
-    <t>AppreciateUnAppreciateOwnPost</t>
-  </si>
-  <si>
     <t>OPQA-379|OPQA-381</t>
   </si>
   <si>
     <t>Verify that user is able to Appreciate/Un Appreciate their own post</t>
   </si>
   <si>
-    <t>PostTitleProfanityWordCheckTest</t>
-  </si>
-  <si>
     <t>CREATE POST:Verfiy that profanity words are not allowed in post title</t>
   </si>
   <si>
     <t>CREATE POST:Verfiy that profanity words are not allowed in post content</t>
   </si>
   <si>
-    <t>EditPostContentProfanityWordCheckTest</t>
-  </si>
-  <si>
     <t>EDIT POST:Verfiy that profanity words are not allowed in post content</t>
   </si>
   <si>
-    <t>EditPostTitleProfanityWordCheckTest</t>
-  </si>
-  <si>
     <t>EDIT POST:Verfiy that profanity words are not allowed in post title</t>
   </si>
   <si>
-    <t>EditPostTitleMinMaxLengthValidation</t>
-  </si>
-  <si>
-    <t>EidtPostContentMinMaxLenValidation</t>
-  </si>
-  <si>
-    <t>AppreciateUnAppreciateOthersPost</t>
-  </si>
-  <si>
     <t>OPQA-342|OPQA-359</t>
   </si>
   <si>
     <t>Verify that user is able to Appreciate/Un Appreciate their others post</t>
   </si>
   <si>
-    <t>CreateAndEditPost</t>
-  </si>
-  <si>
     <t>OPQA-382|OPQA-388|OPQA-406|OPQA-372</t>
   </si>
   <si>
@@ -455,54 +338,36 @@
     <t>drug delivery systems</t>
   </si>
   <si>
-    <t>VerifyPostRecordDetails</t>
-  </si>
-  <si>
     <t>OPQA-370</t>
   </si>
   <si>
     <t>Verify that user contributed articles display the information about the author</t>
   </si>
   <si>
-    <t>SeacrhAndViewOwnPost</t>
-  </si>
-  <si>
     <t>OPQA-415</t>
   </si>
   <si>
     <t>Verify that user is able to search the  posts a user authored themselves and view them.</t>
   </si>
   <si>
-    <t>SeacrhAndViewOthersPost</t>
-  </si>
-  <si>
     <t>OPQA-416</t>
   </si>
   <si>
     <t>Verify that user is able to search the posts of others and view them.</t>
   </si>
   <si>
-    <t>CancelPostCreation</t>
-  </si>
-  <si>
     <t>OPQA-376</t>
   </si>
   <si>
     <t>Veirfy that user is able to cancel the post</t>
   </si>
   <si>
-    <t>CreatePostWithExternalLink</t>
-  </si>
-  <si>
     <t>Verify that the user is able to add external links to the post and publish it.</t>
   </si>
   <si>
     <t>OPQA-367</t>
   </si>
   <si>
-    <t>EditCommentsMinMaxValidationTest</t>
-  </si>
-  <si>
     <t>OPQA-244</t>
   </si>
   <si>
@@ -512,9 +377,6 @@
     <t>SKIP</t>
   </si>
   <si>
-    <t>PostContentProfanityWordCheckTest</t>
-  </si>
-  <si>
     <t>OPQA-1273</t>
   </si>
   <si>
@@ -581,66 +443,33 @@
     <t>OPQA-1289</t>
   </si>
   <si>
-    <t>VerifyStatsOfOthersPost</t>
-  </si>
-  <si>
     <t>OPQA-424|OPQA-426</t>
   </si>
   <si>
     <t>Verify that user is able to view the comment and like counts on posts created by others</t>
   </si>
   <si>
-    <t>VerifyStatsOfOwnPost</t>
-  </si>
-  <si>
     <t>OPQA-423|OPQA-425</t>
   </si>
   <si>
     <t>Verify that user is able to view the comment and like counts on own posts</t>
   </si>
   <si>
-    <t>FollowUnfollowPostsAuthor</t>
-  </si>
-  <si>
     <t>Veirfy that the user is able to follow the author of the post directly from the post</t>
   </si>
   <si>
     <t>OPQA-427</t>
   </si>
   <si>
-    <t>CommentOnUsersOwnPost</t>
-  </si>
-  <si>
     <t>Verify that the user is able to comment on the post a user authored themselves.</t>
   </si>
   <si>
     <t>OPQA-377</t>
   </si>
   <si>
-    <t>CommentOnOtherUsersPost</t>
-  </si>
-  <si>
     <t>Verify that user is able to add comments on the posts of others.</t>
   </si>
   <si>
-    <t>ShareOthersPostInFB</t>
-  </si>
-  <si>
-    <t>ShareOthersPostOnLI</t>
-  </si>
-  <si>
-    <t>ShareOthersPostOnTwitter</t>
-  </si>
-  <si>
-    <t>ShareOwnPostInFB</t>
-  </si>
-  <si>
-    <t>ShareOwnPostOnLI</t>
-  </si>
-  <si>
-    <t>ShareOwnPostOnTwitter</t>
-  </si>
-  <si>
     <t>OPQA-1307</t>
   </si>
   <si>
@@ -677,9 +506,6 @@
     <t>Verify that user is able to share their posts on Twitter</t>
   </si>
   <si>
-    <t>FlagUnflagUserPost</t>
-  </si>
-  <si>
     <t>OPQA-1074|OPQA-1075</t>
   </si>
   <si>
@@ -692,28 +518,16 @@
     <t> OPQA-1076</t>
   </si>
   <si>
-    <t>DeleteUserPost</t>
-  </si>
-  <si>
-    <t>VerifySavePostAsDraft</t>
-  </si>
-  <si>
     <t>OPQA-1195,OPQA-1313</t>
   </si>
   <si>
     <t>Verfify that user is able to save the post as a draft</t>
   </si>
   <si>
-    <t>VerifyAccessAndEditDraftPost</t>
-  </si>
-  <si>
     <t>OPQA-1312</t>
   </si>
   <si>
     <t>Verfiy that user is able to access and edit the draft posts from their profile</t>
-  </si>
-  <si>
-    <t>VerifyEditDraftPostFromModalWindow</t>
   </si>
   <si>
     <t>OPQA-1196</t>
@@ -729,12 +543,6 @@
     <t>OPQA-1197</t>
   </si>
   <si>
-    <t>VerifyDraftPostDisplayInUserOwnProfile</t>
-  </si>
-  <si>
-    <t>DeleteDraftPostFromProfile</t>
-  </si>
-  <si>
     <t>OPQA-1090|OPQA-1201</t>
   </si>
   <si>
@@ -742,9 +550,6 @@
   </si>
   <si>
     <t>OPQA-385|OPQA-364</t>
-  </si>
-  <si>
-    <t>VerifyPublishPostDisplayed</t>
   </si>
   <si>
     <t>OPQA-1190</t>
@@ -760,12 +565,6 @@
     <t>OPQA-1198</t>
   </si>
   <si>
-    <t>VerifyDraftPostTabDisplayForZeroDrafts</t>
-  </si>
-  <si>
-    <t>DeleteDraftPostFromPostModal</t>
-  </si>
-  <si>
     <t>OPQA-1200</t>
   </si>
   <si>
@@ -779,21 +578,12 @@
     <t>OPQA-1199</t>
   </si>
   <si>
-    <t>VerifyPostTitleDisplayInDraftSection</t>
-  </si>
-  <si>
-    <t>AddExternalLinksToComments</t>
-  </si>
-  <si>
     <t>OPQA-1092</t>
   </si>
   <si>
     <t>Verfiy that user is able to add external links to the comment</t>
   </si>
   <si>
-    <t>AddInternalLinksToComments</t>
-  </si>
-  <si>
     <t>OPQA-1093</t>
   </si>
   <si>
@@ -813,6 +603,216 @@
   </si>
   <si>
     <t>OPQA-284|OPQA-292</t>
+  </si>
+  <si>
+    <t>Authoring10</t>
+  </si>
+  <si>
+    <t>Authoring11</t>
+  </si>
+  <si>
+    <t>Authoring12</t>
+  </si>
+  <si>
+    <t>Authoring13</t>
+  </si>
+  <si>
+    <t>Authoring14</t>
+  </si>
+  <si>
+    <t>Authoring15</t>
+  </si>
+  <si>
+    <t>Authoring16</t>
+  </si>
+  <si>
+    <t>Authoring17</t>
+  </si>
+  <si>
+    <t>Authoring18</t>
+  </si>
+  <si>
+    <t>Authoring19</t>
+  </si>
+  <si>
+    <t>Authoring20</t>
+  </si>
+  <si>
+    <t>Authoring21</t>
+  </si>
+  <si>
+    <t>Authoring22</t>
+  </si>
+  <si>
+    <t>Authoring23</t>
+  </si>
+  <si>
+    <t>Authoring24</t>
+  </si>
+  <si>
+    <t>Authoring25</t>
+  </si>
+  <si>
+    <t>Authoring26</t>
+  </si>
+  <si>
+    <t>Authoring27</t>
+  </si>
+  <si>
+    <t>Authoring28</t>
+  </si>
+  <si>
+    <t>Authoring29</t>
+  </si>
+  <si>
+    <t>Authoring30</t>
+  </si>
+  <si>
+    <t>Authoring31</t>
+  </si>
+  <si>
+    <t>Authoring32</t>
+  </si>
+  <si>
+    <t>Authoring33</t>
+  </si>
+  <si>
+    <t>Authoring34</t>
+  </si>
+  <si>
+    <t>Authoring35</t>
+  </si>
+  <si>
+    <t>Authoring36</t>
+  </si>
+  <si>
+    <t>Authoring37</t>
+  </si>
+  <si>
+    <t>Authoring38</t>
+  </si>
+  <si>
+    <t>Authoring39</t>
+  </si>
+  <si>
+    <t>Authoring40</t>
+  </si>
+  <si>
+    <t>Authoring41</t>
+  </si>
+  <si>
+    <t>Authoring42</t>
+  </si>
+  <si>
+    <t>Authoring43</t>
+  </si>
+  <si>
+    <t>Authoring44</t>
+  </si>
+  <si>
+    <t>Authoring45</t>
+  </si>
+  <si>
+    <t>Authoring46</t>
+  </si>
+  <si>
+    <t>Authoring47</t>
+  </si>
+  <si>
+    <t>Authoring48</t>
+  </si>
+  <si>
+    <t>Authoring49</t>
+  </si>
+  <si>
+    <t>Authoring50</t>
+  </si>
+  <si>
+    <t>Authoring51</t>
+  </si>
+  <si>
+    <t>Authoring52</t>
+  </si>
+  <si>
+    <t>Authoring53</t>
+  </si>
+  <si>
+    <t>Authoring54</t>
+  </si>
+  <si>
+    <t>Authoring55</t>
+  </si>
+  <si>
+    <t>Authoring56</t>
+  </si>
+  <si>
+    <t>Authoring57</t>
+  </si>
+  <si>
+    <t>Authoring58</t>
+  </si>
+  <si>
+    <t>Authoring59</t>
+  </si>
+  <si>
+    <t>Authoring60</t>
+  </si>
+  <si>
+    <t>Authoring61</t>
+  </si>
+  <si>
+    <t>Authoring62</t>
+  </si>
+  <si>
+    <t>Authoring63</t>
+  </si>
+  <si>
+    <t>Authoring64</t>
+  </si>
+  <si>
+    <t>Authoring65</t>
+  </si>
+  <si>
+    <t>Authoring66</t>
+  </si>
+  <si>
+    <t>Authoring67</t>
+  </si>
+  <si>
+    <t>Authoring68</t>
+  </si>
+  <si>
+    <t>Authoring69</t>
+  </si>
+  <si>
+    <t>Authoring70</t>
+  </si>
+  <si>
+    <t>Authoring1</t>
+  </si>
+  <si>
+    <t>Authoring2</t>
+  </si>
+  <si>
+    <t>Authoring3</t>
+  </si>
+  <si>
+    <t>Authoring4</t>
+  </si>
+  <si>
+    <t>Authoring5</t>
+  </si>
+  <si>
+    <t>Authoring6</t>
+  </si>
+  <si>
+    <t>Authoring7</t>
+  </si>
+  <si>
+    <t>Authoring8</t>
+  </si>
+  <si>
+    <t>Authoring9</t>
   </si>
 </sst>
 </file>
@@ -947,7 +947,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -985,7 +985,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1286,13 +1285,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
@@ -1304,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>1</v>
@@ -1318,1192 +1317,1192 @@
     </row>
     <row r="2" spans="1:5" ht="25.5">
       <c r="A2" s="18" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>257</v>
+        <v>187</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="25.5">
       <c r="A3" s="18" t="s">
-        <v>50</v>
+        <v>252</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>259</v>
+        <v>189</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="25.5">
       <c r="A4" s="18" t="s">
-        <v>52</v>
+        <v>253</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>256</v>
+        <v>186</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="18" t="s">
-        <v>54</v>
+        <v>254</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="18" t="s">
-        <v>57</v>
+        <v>255</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="25.5">
       <c r="A7" s="18" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>63</v>
+        <v>257</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>161</v>
+        <v>115</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>65</v>
+        <v>258</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="18" t="s">
-        <v>68</v>
+        <v>259</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="18" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
-        <v>74</v>
+        <v>191</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="18" t="s">
-        <v>77</v>
+        <v>192</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
-        <v>79</v>
+        <v>193</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>81</v>
+        <v>194</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>164</v>
+        <v>118</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>83</v>
+        <v>195</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>165</v>
+        <v>119</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>255</v>
+        <v>196</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>185</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="18" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>166</v>
+        <v>120</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="18" t="s">
-        <v>89</v>
+        <v>198</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="18" t="s">
-        <v>91</v>
+        <v>199</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>93</v>
+        <v>200</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>169</v>
+        <v>123</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>95</v>
+        <v>201</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>171</v>
+        <v>125</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>170</v>
+        <v>124</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>96</v>
+        <v>202</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>258</v>
+        <v>188</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="18" t="s">
-        <v>98</v>
+        <v>203</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="18" t="s">
-        <v>101</v>
+        <v>204</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="25.5">
       <c r="A28" s="18" t="s">
-        <v>110</v>
+        <v>207</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>172</v>
+        <v>126</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="25.5">
       <c r="A29" s="18" t="s">
-        <v>112</v>
+        <v>208</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>113</v>
+        <v>85</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>115</v>
+        <v>209</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="25.5">
       <c r="A31" s="18" t="s">
-        <v>118</v>
+        <v>210</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
       <c r="D31" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="25.5">
       <c r="A32" s="18" t="s">
-        <v>120</v>
+        <v>211</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>176</v>
+        <v>130</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>122</v>
+        <v>212</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="D34" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>180</v>
+        <v>134</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>127</v>
+        <v>94</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>128</v>
+        <v>215</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>130</v>
+        <v>216</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>178</v>
+        <v>132</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="25.5">
       <c r="A38" s="18" t="s">
-        <v>132</v>
+        <v>217</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="25.5">
       <c r="A39" s="18" t="s">
-        <v>133</v>
+        <v>218</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>174</v>
+        <v>128</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="18" t="s">
-        <v>134</v>
+        <v>219</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="D40" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B41" s="19" t="s">
+      <c r="C48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="D48" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B49" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="C49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B56" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B57" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B58" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="B59" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="8" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D43" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>151</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D45" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D47" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="s">
+      <c r="D59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="B60" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="30">
+      <c r="A64" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45">
+      <c r="A66" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="30">
+      <c r="A69" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="C71" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D48" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D49" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D50" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D51" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>236</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D52" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D54" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D61" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D62" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="30">
-      <c r="A64" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D64" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="45">
-      <c r="A66" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D66" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="30">
-      <c r="A69" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="D71" s="18" t="s">
         <v>3</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2580,13 +2579,13 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>2</v>
@@ -2597,7 +2596,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2609,7 +2608,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2637,16 +2636,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2657,10 +2656,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>46</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2672,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2698,10 +2697,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -2712,86 +2711,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2803,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2878,7 +2877,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2889,7 +2888,7 @@
         <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>14</v>
@@ -2926,16 +2925,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -2949,19 +2948,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -2988,10 +2987,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
       <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -3002,86 +3001,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3108,10 +3107,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -3122,44 +3121,44 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3184,10 +3183,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>24</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -3198,86 +3197,86 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>26</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75">
       <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75">
       <c r="A6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3303,16 +3302,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -3326,19 +3325,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="10">
         <v>1600</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3364,10 +3363,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>2</v>
@@ -3378,44 +3377,44 @@
     </row>
     <row r="2" spans="1:4" ht="15.75">
       <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45">
       <c r="A4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing the Suite and module name for watchlist
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="260">
   <si>
     <t>TCID</t>
   </si>
@@ -819,6 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1291,11 +1292,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2573,8 +2574,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2627,11 +2628,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2690,9 +2691,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2808,10 +2809,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2849,12 +2850,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2916,11 +2917,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2979,10 +2980,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3099,10 +3100,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3176,9 +3177,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3294,10 +3295,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3360,10 +3361,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Framework changes made to search module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/C suite.xlsx
+++ b/src/test/resources/xls/C suite.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="260">
   <si>
     <t>TCID</t>
   </si>
@@ -819,6 +819,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="10">
     <font>
       <sz val="11"/>
@@ -1291,11 +1292,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.8046875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
@@ -2573,8 +2574,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="56" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="56.0" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2627,11 +2628,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2690,9 +2691,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="58.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2808,10 +2809,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2849,12 +2850,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2916,11 +2917,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="47.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2979,10 +2980,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="54.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="11" customFormat="1">
@@ -3099,10 +3100,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="61.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3176,9 +3177,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="59.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3294,10 +3295,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="68.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="68.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3360,10 +3361,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="35.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>